<commit_message>
resumen del codigo, post, carusel y mejora al menu desplegable
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva - copia.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva - copia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\blog centro agroturistico\Bitacioras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D031E46B-A4AD-48BE-85F5-E030E9684861}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6411244E-23B7-4993-B6F6-5AE656DEE7C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -871,18 +871,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>solución de bug: antes cuando la ventana se hacia muy delgada y luego volvía a la normalidad lo post obtendrían la clase de 2 columnas aun que esto no fueran tan largos
-el espaciado dentro de las publicaciones ahora es mas uniforme
-agrege una funcion que elimina renglones en blanco en caso que se pongan por accidente al publicar un post
-ahora si hay 2 poblicaciones de diferente tamaño la mas pequeña ya no se estirara, aun que esto tal vez cambien en un futuro
-la parte inferior ahora esta fijada abajo del todo y no se depegara el borde
-cuando estas en movil la parte inferior adopta una forma mas compacta</t>
-  </si>
-  <si>
-    <t>al aplicar la funcion que quita espacio me di cuenta que el boton de descarga se rompia, era ovio ya que este esta echo con sinta y aduras penas funcionaba antes
-estavez lo volvi a rehacer con un codigo mas intuitivo y bien comentado esto es en lo que mas tiempo estuve ocupado</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1009,12 +997,21 @@
   <si>
     <t>solo fue diseño entonces no tuve ningun problema hoy, aun que hubo un fallo de internet en la oficina una rato</t>
   </si>
+  <si>
+    <t>al estar simplificando el codigo el visor de imágenes dejo de funcionar y por ende tuve que buscar la forma de desactivar el que ya venia por defecto, ah otra cosas devez en cuando se iva el internet pero no por tanto tiempo</t>
+  </si>
+  <si>
+    <t>cuando cambiaba de pagina se quedaba el fondo borroso, tambien los botones de descarga se hiba asi que retire la funcion que hacia que solo se cargara un trozo de la pagina
+resumi la función que pasaba de pagina en el carusel, ahora es mas simple
+combine la función de agregar botones y la de agregar la biblioteca de visualización de imágenes, ademas puse variables globales a las cosas relacionadas con posts 
+ encontré la forma de desactivar el visor de imágenes por defecto de Blogger y lo inclui a la documentacion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1281,6 +1278,12 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -2383,7 +2386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="278">
+  <cellXfs count="279">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2860,6 +2863,99 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="82" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2893,18 +2989,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2914,86 +2998,83 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3001,12 +3082,18 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3016,89 +3103,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3112,95 +3205,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4187,56 +4193,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="193"/>
-      <c r="D3" s="193"/>
-      <c r="E3" s="194"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="170"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="195" t="s">
+      <c r="B4" s="171" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="196"/>
-      <c r="D4" s="196"/>
-      <c r="E4" s="197"/>
+      <c r="C4" s="172"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="173"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="198" t="s">
+      <c r="B5" s="174" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="199"/>
-      <c r="D5" s="199"/>
-      <c r="E5" s="200"/>
+      <c r="C5" s="175"/>
+      <c r="D5" s="175"/>
+      <c r="E5" s="176"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="195" t="s">
+      <c r="B6" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
-      <c r="E6" s="197"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="173"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="192" t="s">
+      <c r="B7" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="193"/>
-      <c r="D7" s="193"/>
-      <c r="E7" s="194"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="170"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4248,45 +4254,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="201" t="s">
+      <c r="D8" s="177" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="202"/>
+      <c r="E8" s="178"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="203" t="s">
+      <c r="B9" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="204"/>
-      <c r="D9" s="204"/>
-      <c r="E9" s="205"/>
+      <c r="C9" s="180"/>
+      <c r="D9" s="180"/>
+      <c r="E9" s="181"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="206" t="s">
+      <c r="B10" s="182" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="207"/>
-      <c r="D10" s="207"/>
-      <c r="E10" s="208"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="184"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="184" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="185"/>
-      <c r="D11" s="185"/>
-      <c r="E11" s="186"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="175" t="s">
+      <c r="B12" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="176"/>
-      <c r="D12" s="177"/>
-      <c r="E12" s="178"/>
+      <c r="C12" s="165"/>
+      <c r="D12" s="166"/>
+      <c r="E12" s="167"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4297,84 +4303,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="166" t="s">
+      <c r="B14" s="197" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="167"/>
-      <c r="D14" s="167"/>
-      <c r="E14" s="168"/>
+      <c r="C14" s="198"/>
+      <c r="D14" s="198"/>
+      <c r="E14" s="199"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="169" t="s">
+      <c r="B15" s="200" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="170"/>
-      <c r="D15" s="170"/>
-      <c r="E15" s="171"/>
+      <c r="C15" s="201"/>
+      <c r="D15" s="201"/>
+      <c r="E15" s="202"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="169" t="s">
+      <c r="B16" s="200" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="170"/>
-      <c r="D16" s="170"/>
-      <c r="E16" s="171"/>
+      <c r="C16" s="201"/>
+      <c r="D16" s="201"/>
+      <c r="E16" s="202"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="179" t="s">
+      <c r="B17" s="206" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="180"/>
-      <c r="D17" s="180"/>
-      <c r="E17" s="181"/>
+      <c r="C17" s="207"/>
+      <c r="D17" s="207"/>
+      <c r="E17" s="208"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="169" t="s">
+      <c r="B18" s="200" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="170"/>
-      <c r="D18" s="170"/>
-      <c r="E18" s="171"/>
+      <c r="C18" s="201"/>
+      <c r="D18" s="201"/>
+      <c r="E18" s="202"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="169" t="s">
+      <c r="B19" s="200" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="170"/>
-      <c r="D19" s="170"/>
-      <c r="E19" s="171"/>
+      <c r="C19" s="201"/>
+      <c r="D19" s="201"/>
+      <c r="E19" s="202"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="172" t="s">
+      <c r="B20" s="203" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="173"/>
-      <c r="D20" s="173"/>
-      <c r="E20" s="174"/>
+      <c r="C20" s="204"/>
+      <c r="D20" s="204"/>
+      <c r="E20" s="205"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="175" t="s">
+      <c r="B21" s="164" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="176"/>
-      <c r="D21" s="177"/>
-      <c r="E21" s="178"/>
+      <c r="C21" s="165"/>
+      <c r="D21" s="166"/>
+      <c r="E21" s="167"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="184" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="185"/>
-      <c r="D22" s="185" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="186"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="187"/>
-      <c r="C23" s="188"/>
-      <c r="D23" s="188"/>
-      <c r="E23" s="189"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4383,10 +4389,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="190" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="191"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4396,8 +4402,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="182"/>
-      <c r="E25" s="183"/>
+      <c r="D25" s="193"/>
+      <c r="E25" s="194"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4406,8 +4412,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="182"/>
-      <c r="E26" s="183"/>
+      <c r="D26" s="193"/>
+      <c r="E26" s="194"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4416,8 +4422,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="182"/>
-      <c r="E27" s="183"/>
+      <c r="D27" s="193"/>
+      <c r="E27" s="194"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4426,8 +4432,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="182"/>
-      <c r="E28" s="183"/>
+      <c r="D28" s="193"/>
+      <c r="E28" s="194"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4436,10 +4442,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="182" t="s">
+      <c r="D29" s="193" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="183" t="s">
+      <c r="E29" s="194" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4450,10 +4456,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="182" t="s">
+      <c r="D30" s="193" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="183" t="s">
+      <c r="E30" s="194" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4464,8 +4470,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="182"/>
-      <c r="E31" s="183"/>
+      <c r="D31" s="193"/>
+      <c r="E31" s="194"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4474,10 +4480,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="182" t="s">
+      <c r="D32" s="193" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="183" t="s">
+      <c r="E32" s="194" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4488,8 +4494,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="182"/>
-      <c r="E33" s="183"/>
+      <c r="D33" s="193"/>
+      <c r="E33" s="194"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4498,8 +4504,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="182"/>
-      <c r="E34" s="183"/>
+      <c r="D34" s="193"/>
+      <c r="E34" s="194"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4508,8 +4514,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="182"/>
-      <c r="E35" s="183"/>
+      <c r="D35" s="193"/>
+      <c r="E35" s="194"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4518,8 +4524,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="182"/>
-      <c r="E36" s="183"/>
+      <c r="D36" s="193"/>
+      <c r="E36" s="194"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4528,8 +4534,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="182"/>
-      <c r="E37" s="183"/>
+      <c r="D37" s="193"/>
+      <c r="E37" s="194"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4538,8 +4544,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="182"/>
-      <c r="E38" s="183"/>
+      <c r="D38" s="193"/>
+      <c r="E38" s="194"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4548,8 +4554,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="182"/>
-      <c r="E39" s="183"/>
+      <c r="D39" s="193"/>
+      <c r="E39" s="194"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4558,8 +4564,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="182"/>
-      <c r="E40" s="183"/>
+      <c r="D40" s="193"/>
+      <c r="E40" s="194"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4568,8 +4574,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="182"/>
-      <c r="E41" s="183"/>
+      <c r="D41" s="193"/>
+      <c r="E41" s="194"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4578,8 +4584,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="182"/>
-      <c r="E42" s="183"/>
+      <c r="D42" s="193"/>
+      <c r="E42" s="194"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4588,10 +4594,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="182" t="s">
+      <c r="D43" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="183" t="s">
+      <c r="E43" s="194" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4602,8 +4608,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="182"/>
-      <c r="E44" s="183"/>
+      <c r="D44" s="193"/>
+      <c r="E44" s="194"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4612,8 +4618,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="182"/>
-      <c r="E45" s="183"/>
+      <c r="D45" s="193"/>
+      <c r="E45" s="194"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4622,8 +4628,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="182"/>
-      <c r="E46" s="183"/>
+      <c r="D46" s="193"/>
+      <c r="E46" s="194"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4632,10 +4638,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="182" t="s">
+      <c r="D47" s="193" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="183" t="s">
+      <c r="E47" s="194" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4646,8 +4652,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="182"/>
-      <c r="E48" s="183"/>
+      <c r="D48" s="193"/>
+      <c r="E48" s="194"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4656,10 +4662,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="182" t="s">
+      <c r="D49" s="193" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="183" t="s">
+      <c r="E49" s="194" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4670,10 +4676,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="182" t="s">
+      <c r="D50" s="193" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="183" t="s">
+      <c r="E50" s="194" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4684,10 +4690,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="182" t="s">
+      <c r="D51" s="193" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="183" t="s">
+      <c r="E51" s="194" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4698,8 +4704,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="182"/>
-      <c r="E52" s="183"/>
+      <c r="D52" s="193"/>
+      <c r="E52" s="194"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4708,8 +4714,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="182"/>
-      <c r="E53" s="183"/>
+      <c r="D53" s="193"/>
+      <c r="E53" s="194"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4718,8 +4724,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="182"/>
-      <c r="E54" s="183"/>
+      <c r="D54" s="193"/>
+      <c r="E54" s="194"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4728,8 +4734,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="182"/>
-      <c r="E55" s="183"/>
+      <c r="D55" s="193"/>
+      <c r="E55" s="194"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4738,8 +4744,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="182"/>
-      <c r="E56" s="183"/>
+      <c r="D56" s="193"/>
+      <c r="E56" s="194"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4748,10 +4754,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="164" t="s">
+      <c r="D57" s="195" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="165" t="s">
+      <c r="E57" s="196" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4769,44 +4775,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4823,6 +4791,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4838,7 +4844,7 @@
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4920,14 +4926,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="193"/>
-      <c r="D3" s="193"/>
-      <c r="E3" s="193"/>
-      <c r="F3" s="193"/>
-      <c r="G3" s="194"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="170"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4949,14 +4955,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="195" t="s">
+      <c r="B4" s="171" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="196"/>
-      <c r="D4" s="196"/>
-      <c r="E4" s="196"/>
-      <c r="F4" s="196"/>
-      <c r="G4" s="197"/>
+      <c r="C4" s="172"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="172"/>
+      <c r="F4" s="172"/>
+      <c r="G4" s="173"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4978,14 +4984,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="192" t="s">
+      <c r="B5" s="168" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="193"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
-      <c r="G5" s="194"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -5007,14 +5013,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="195" t="s">
+      <c r="B6" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
-      <c r="E6" s="196"/>
-      <c r="F6" s="196"/>
-      <c r="G6" s="197"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="173"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -5036,14 +5042,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="192" t="s">
+      <c r="B7" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="193"/>
-      <c r="D7" s="193"/>
-      <c r="E7" s="193"/>
-      <c r="F7" s="193"/>
-      <c r="G7" s="194"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5239,16 +5245,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="217">
+      <c r="B14" s="215">
         <v>2557356</v>
       </c>
-      <c r="C14" s="238"/>
-      <c r="D14" s="212"/>
-      <c r="E14" s="236" t="s">
+      <c r="C14" s="220"/>
+      <c r="D14" s="216"/>
+      <c r="E14" s="217" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="216"/>
-      <c r="G14" s="237"/>
+      <c r="F14" s="218"/>
+      <c r="G14" s="219"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5320,20 +5326,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="217" t="s">
+      <c r="B17" s="215" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="212"/>
+      <c r="C17" s="216"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>6</v>
       </c>
-      <c r="F17" s="239" t="s">
+      <c r="F17" s="221" t="s">
         <v>200</v>
       </c>
-      <c r="G17" s="240"/>
+      <c r="G17" s="222"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5401,20 +5407,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="217" t="s">
+      <c r="B20" s="215" t="s">
         <v>203</v>
       </c>
-      <c r="C20" s="212"/>
+      <c r="C20" s="216"/>
       <c r="D20" s="108" t="s">
         <v>201</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="241" t="s">
         <v>202</v>
       </c>
-      <c r="G20" s="214"/>
+      <c r="G20" s="242"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5456,14 +5462,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="233" t="s">
+      <c r="B22" s="212" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="234"/>
-      <c r="D22" s="234"/>
-      <c r="E22" s="234"/>
-      <c r="F22" s="234"/>
-      <c r="G22" s="235"/>
+      <c r="C22" s="213"/>
+      <c r="D22" s="213"/>
+      <c r="E22" s="213"/>
+      <c r="F22" s="213"/>
+      <c r="G22" s="214"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5488,17 +5494,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="211" t="s">
+      <c r="C23" s="240" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="212"/>
+      <c r="D23" s="216"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="241" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="214"/>
+      <c r="G23" s="242"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5642,10 +5648,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="241" t="s">
+      <c r="F28" s="209" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="242"/>
+      <c r="G28" s="210"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5672,8 +5678,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="241"/>
-      <c r="G29" s="242"/>
+      <c r="F29" s="209"/>
+      <c r="G29" s="210"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -6011,10 +6017,10 @@
       <c r="Y39" s="18"/>
     </row>
     <row r="40" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="209" t="s">
-        <v>226</v>
-      </c>
-      <c r="C40" s="210"/>
+      <c r="B40" s="235" t="s">
+        <v>224</v>
+      </c>
+      <c r="C40" s="236"/>
       <c r="D40" s="161">
         <v>45735</v>
       </c>
@@ -6022,10 +6028,10 @@
         <v>45735</v>
       </c>
       <c r="F40" s="160" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G40" s="160" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
@@ -6047,21 +6053,21 @@
       <c r="Y40" s="18"/>
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="209" t="s">
+      <c r="B41" s="235" t="s">
+        <v>227</v>
+      </c>
+      <c r="C41" s="236"/>
+      <c r="D41" s="161">
+        <v>45736</v>
+      </c>
+      <c r="E41" s="161">
+        <v>45736</v>
+      </c>
+      <c r="F41" s="160" t="s">
         <v>205</v>
       </c>
-      <c r="C41" s="210"/>
-      <c r="D41" s="161">
-        <v>45721</v>
-      </c>
-      <c r="E41" s="161">
-        <v>45721</v>
-      </c>
-      <c r="F41" s="160" t="s">
-        <v>207</v>
-      </c>
       <c r="G41" s="160" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
@@ -6083,10 +6089,10 @@
       <c r="Y41" s="18"/>
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="209" t="s">
-        <v>209</v>
-      </c>
-      <c r="C42" s="210"/>
+      <c r="B42" s="235" t="s">
+        <v>207</v>
+      </c>
+      <c r="C42" s="236"/>
       <c r="D42" s="161">
         <v>45722</v>
       </c>
@@ -6094,10 +6100,10 @@
         <v>45722</v>
       </c>
       <c r="F42" s="160" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6119,10 +6125,10 @@
       <c r="Y42" s="18"/>
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="209" t="s">
-        <v>211</v>
-      </c>
-      <c r="C43" s="210"/>
+      <c r="B43" s="235" t="s">
+        <v>209</v>
+      </c>
+      <c r="C43" s="236"/>
       <c r="D43" s="161">
         <v>45723</v>
       </c>
@@ -6130,10 +6136,10 @@
         <v>45723</v>
       </c>
       <c r="F43" s="160" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G43" s="160" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H43" s="20"/>
       <c r="I43" s="18"/>
@@ -6155,8 +6161,8 @@
       <c r="Y43" s="18"/>
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="209"/>
-      <c r="C44" s="210"/>
+      <c r="B44" s="235"/>
+      <c r="C44" s="236"/>
       <c r="D44" s="161"/>
       <c r="E44" s="161"/>
       <c r="F44" s="160"/>
@@ -6181,8 +6187,8 @@
       <c r="Y44" s="18"/>
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="209"/>
-      <c r="C45" s="210"/>
+      <c r="B45" s="235"/>
+      <c r="C45" s="236"/>
       <c r="D45" s="161"/>
       <c r="E45" s="161"/>
       <c r="F45" s="160"/>
@@ -6207,10 +6213,10 @@
       <c r="Y45" s="18"/>
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="209" t="s">
-        <v>213</v>
-      </c>
-      <c r="C46" s="210"/>
+      <c r="B46" s="235" t="s">
+        <v>211</v>
+      </c>
+      <c r="C46" s="236"/>
       <c r="D46" s="161">
         <v>45726</v>
       </c>
@@ -6218,10 +6224,10 @@
         <v>45726</v>
       </c>
       <c r="F46" s="160" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G46" s="160" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="18"/>
@@ -6243,10 +6249,10 @@
       <c r="Y46" s="18"/>
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="209" t="s">
-        <v>215</v>
-      </c>
-      <c r="C47" s="210"/>
+      <c r="B47" s="235" t="s">
+        <v>213</v>
+      </c>
+      <c r="C47" s="236"/>
       <c r="D47" s="161">
         <v>45727</v>
       </c>
@@ -6254,10 +6260,10 @@
         <v>45727</v>
       </c>
       <c r="F47" s="160" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6279,10 +6285,10 @@
       <c r="Y47" s="18"/>
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="209" t="s">
-        <v>219</v>
-      </c>
-      <c r="C48" s="210"/>
+      <c r="B48" s="235" t="s">
+        <v>217</v>
+      </c>
+      <c r="C48" s="236"/>
       <c r="D48" s="161">
         <v>45728</v>
       </c>
@@ -6290,10 +6296,10 @@
         <v>45728</v>
       </c>
       <c r="F48" s="160" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G48" s="160" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
@@ -6315,10 +6321,10 @@
       <c r="Y48" s="18"/>
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="209" t="s">
-        <v>217</v>
-      </c>
-      <c r="C49" s="210"/>
+      <c r="B49" s="235" t="s">
+        <v>215</v>
+      </c>
+      <c r="C49" s="236"/>
       <c r="D49" s="161">
         <v>45729</v>
       </c>
@@ -6326,10 +6332,10 @@
         <v>45729</v>
       </c>
       <c r="F49" s="160" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6351,10 +6357,10 @@
       <c r="Y49" s="18"/>
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="209" t="s">
-        <v>221</v>
-      </c>
-      <c r="C50" s="210"/>
+      <c r="B50" s="235" t="s">
+        <v>219</v>
+      </c>
+      <c r="C50" s="236"/>
       <c r="D50" s="161">
         <v>45730</v>
       </c>
@@ -6362,10 +6368,10 @@
         <v>45730</v>
       </c>
       <c r="F50" s="160" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6387,8 +6393,8 @@
       <c r="Y50" s="18"/>
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="209"/>
-      <c r="C51" s="210"/>
+      <c r="B51" s="235"/>
+      <c r="C51" s="236"/>
       <c r="D51" s="161"/>
       <c r="E51" s="161"/>
       <c r="F51" s="160"/>
@@ -6413,8 +6419,8 @@
       <c r="Y51" s="18"/>
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="209"/>
-      <c r="C52" s="210"/>
+      <c r="B52" s="235"/>
+      <c r="C52" s="236"/>
       <c r="D52" s="161"/>
       <c r="E52" s="161"/>
       <c r="F52" s="160"/>
@@ -6439,10 +6445,10 @@
       <c r="Y52" s="18"/>
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="209" t="s">
-        <v>223</v>
-      </c>
-      <c r="C53" s="210"/>
+      <c r="B53" s="235" t="s">
+        <v>221</v>
+      </c>
+      <c r="C53" s="236"/>
       <c r="D53" s="161">
         <v>45733</v>
       </c>
@@ -6450,10 +6456,10 @@
         <v>45733</v>
       </c>
       <c r="F53" s="160" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G53" s="160" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H53" s="20"/>
       <c r="I53" s="18"/>
@@ -6475,10 +6481,10 @@
       <c r="Y53" s="18"/>
     </row>
     <row r="54" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="209" t="s">
-        <v>225</v>
-      </c>
-      <c r="C54" s="210"/>
+      <c r="B54" s="235" t="s">
+        <v>223</v>
+      </c>
+      <c r="C54" s="236"/>
       <c r="D54" s="161">
         <v>45734</v>
       </c>
@@ -6508,7 +6514,7 @@
     </row>
     <row r="55" spans="2:26" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="27"/>
-      <c r="C55" s="20"/>
+      <c r="C55" s="278"/>
       <c r="D55" s="20"/>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
@@ -6561,14 +6567,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="237" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="238"/>
+      <c r="D57" s="238"/>
+      <c r="E57" s="238"/>
+      <c r="F57" s="238"/>
+      <c r="G57" s="239"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6742,7 +6748,7 @@
     </row>
     <row r="63" spans="2:26" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="97" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C63" s="98">
         <v>1</v>
@@ -6827,9 +6833,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="223"/>
-      <c r="C66" s="223"/>
-      <c r="D66" s="223"/>
+      <c r="B66" s="225"/>
+      <c r="C66" s="225"/>
+      <c r="D66" s="225"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6854,11 +6860,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="223"/>
-      <c r="C67" s="223"/>
-      <c r="D67" s="223"/>
+      <c r="B67" s="225"/>
+      <c r="C67" s="225"/>
+      <c r="D67" s="225"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="225" t="s">
+      <c r="F67" s="227" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6883,10 +6889,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="224"/>
-      <c r="C68" s="224"/>
-      <c r="D68" s="224"/>
-      <c r="F68" s="226"/>
+      <c r="B68" s="226"/>
+      <c r="C68" s="226"/>
+      <c r="D68" s="226"/>
+      <c r="F68" s="228"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6909,11 +6915,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="243" t="s">
+      <c r="B69" s="211" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="243"/>
-      <c r="D69" s="243"/>
+      <c r="C69" s="211"/>
+      <c r="D69" s="211"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6965,11 +6971,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="221"/>
-      <c r="C71" s="221"/>
-      <c r="D71" s="221"/>
-      <c r="F71" s="215"/>
-      <c r="G71" s="215"/>
+      <c r="B71" s="223"/>
+      <c r="C71" s="223"/>
+      <c r="D71" s="223"/>
+      <c r="F71" s="243"/>
+      <c r="G71" s="243"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6991,11 +6997,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="222"/>
-      <c r="C72" s="222"/>
-      <c r="D72" s="222"/>
-      <c r="F72" s="216"/>
-      <c r="G72" s="216"/>
+      <c r="B72" s="224"/>
+      <c r="C72" s="224"/>
+      <c r="D72" s="224"/>
+      <c r="F72" s="218"/>
+      <c r="G72" s="218"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -7022,10 +7028,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="243" t="s">
+      <c r="F73" s="211" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="243"/>
+      <c r="G73" s="211"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7103,14 +7109,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="227" t="s">
+      <c r="B76" s="229" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="228"/>
-      <c r="D76" s="228"/>
-      <c r="E76" s="228"/>
-      <c r="F76" s="228"/>
-      <c r="G76" s="229"/>
+      <c r="C76" s="230"/>
+      <c r="D76" s="230"/>
+      <c r="E76" s="230"/>
+      <c r="F76" s="230"/>
+      <c r="G76" s="231"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7132,14 +7138,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="230" t="s">
+      <c r="B77" s="232" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="231"/>
-      <c r="D77" s="231"/>
-      <c r="E77" s="231"/>
-      <c r="F77" s="231"/>
-      <c r="G77" s="232"/>
+      <c r="C77" s="233"/>
+      <c r="D77" s="233"/>
+      <c r="E77" s="233"/>
+      <c r="F77" s="233"/>
+      <c r="G77" s="234"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7170,16 +7176,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7187,23 +7191,25 @@
     <mergeCell ref="B71:D72"/>
     <mergeCell ref="B66:D68"/>
     <mergeCell ref="F67:F68"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
@@ -7327,124 +7333,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="270" t="s">
+      <c r="A1" s="244" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="270"/>
-      <c r="C1" s="270"/>
-      <c r="D1" s="270"/>
-      <c r="E1" s="270"/>
-      <c r="F1" s="270"/>
-      <c r="G1" s="270"/>
-      <c r="H1" s="270"/>
-      <c r="I1" s="270"/>
-      <c r="J1" s="270"/>
-      <c r="K1" s="270"/>
-      <c r="L1" s="270"/>
-      <c r="M1" s="270"/>
-      <c r="N1" s="270"/>
-      <c r="O1" s="270"/>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="270"/>
-      <c r="R1" s="270"/>
-      <c r="S1" s="270"/>
-      <c r="T1" s="270"/>
-      <c r="U1" s="270" t="s">
+      <c r="B1" s="244"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
+      <c r="G1" s="244"/>
+      <c r="H1" s="244"/>
+      <c r="I1" s="244"/>
+      <c r="J1" s="244"/>
+      <c r="K1" s="244"/>
+      <c r="L1" s="244"/>
+      <c r="M1" s="244"/>
+      <c r="N1" s="244"/>
+      <c r="O1" s="244"/>
+      <c r="P1" s="244"/>
+      <c r="Q1" s="244"/>
+      <c r="R1" s="244"/>
+      <c r="S1" s="244"/>
+      <c r="T1" s="244"/>
+      <c r="U1" s="244" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="270"/>
-      <c r="W1" s="270"/>
-      <c r="X1" s="270"/>
+      <c r="V1" s="244"/>
+      <c r="W1" s="244"/>
+      <c r="X1" s="244"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="270"/>
-      <c r="B2" s="270"/>
-      <c r="C2" s="270"/>
-      <c r="D2" s="270"/>
-      <c r="E2" s="270"/>
-      <c r="F2" s="270"/>
-      <c r="G2" s="270"/>
-      <c r="H2" s="270"/>
-      <c r="I2" s="270"/>
-      <c r="J2" s="270"/>
-      <c r="K2" s="270"/>
-      <c r="L2" s="270"/>
-      <c r="M2" s="270"/>
-      <c r="N2" s="270"/>
-      <c r="O2" s="270"/>
-      <c r="P2" s="270"/>
-      <c r="Q2" s="270"/>
-      <c r="R2" s="270"/>
-      <c r="S2" s="270"/>
-      <c r="T2" s="270"/>
-      <c r="U2" s="250" t="s">
+      <c r="A2" s="244"/>
+      <c r="B2" s="244"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="244"/>
+      <c r="E2" s="244"/>
+      <c r="F2" s="244"/>
+      <c r="G2" s="244"/>
+      <c r="H2" s="244"/>
+      <c r="I2" s="244"/>
+      <c r="J2" s="244"/>
+      <c r="K2" s="244"/>
+      <c r="L2" s="244"/>
+      <c r="M2" s="244"/>
+      <c r="N2" s="244"/>
+      <c r="O2" s="244"/>
+      <c r="P2" s="244"/>
+      <c r="Q2" s="244"/>
+      <c r="R2" s="244"/>
+      <c r="S2" s="244"/>
+      <c r="T2" s="244"/>
+      <c r="U2" s="252" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="250"/>
-      <c r="W2" s="250"/>
-      <c r="X2" s="250"/>
+      <c r="V2" s="252"/>
+      <c r="W2" s="252"/>
+      <c r="X2" s="252"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="277"/>
-      <c r="V3" s="277"/>
-      <c r="W3" s="277"/>
-      <c r="X3" s="277"/>
+      <c r="U3" s="253"/>
+      <c r="V3" s="253"/>
+      <c r="W3" s="253"/>
+      <c r="X3" s="253"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="274" t="s">
+      <c r="A4" s="249" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="275"/>
-      <c r="C4" s="275"/>
-      <c r="D4" s="275"/>
-      <c r="E4" s="275"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="275"/>
-      <c r="L4" s="275"/>
-      <c r="M4" s="276"/>
-      <c r="N4" s="274" t="s">
+      <c r="B4" s="250"/>
+      <c r="C4" s="250"/>
+      <c r="D4" s="250"/>
+      <c r="E4" s="250"/>
+      <c r="F4" s="250"/>
+      <c r="G4" s="250"/>
+      <c r="H4" s="250"/>
+      <c r="I4" s="250"/>
+      <c r="J4" s="250"/>
+      <c r="K4" s="250"/>
+      <c r="L4" s="250"/>
+      <c r="M4" s="251"/>
+      <c r="N4" s="249" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="275"/>
-      <c r="P4" s="275"/>
-      <c r="Q4" s="275"/>
-      <c r="R4" s="275"/>
-      <c r="S4" s="275"/>
-      <c r="T4" s="275"/>
-      <c r="U4" s="275"/>
-      <c r="V4" s="275"/>
-      <c r="W4" s="275"/>
-      <c r="X4" s="276"/>
+      <c r="O4" s="250"/>
+      <c r="P4" s="250"/>
+      <c r="Q4" s="250"/>
+      <c r="R4" s="250"/>
+      <c r="S4" s="250"/>
+      <c r="T4" s="250"/>
+      <c r="U4" s="250"/>
+      <c r="V4" s="250"/>
+      <c r="W4" s="250"/>
+      <c r="X4" s="251"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="271"/>
-      <c r="B5" s="272"/>
-      <c r="C5" s="272"/>
-      <c r="D5" s="272"/>
-      <c r="E5" s="272"/>
-      <c r="F5" s="272"/>
-      <c r="G5" s="272"/>
-      <c r="H5" s="272"/>
-      <c r="I5" s="272"/>
-      <c r="J5" s="272"/>
-      <c r="K5" s="272"/>
-      <c r="L5" s="272"/>
-      <c r="M5" s="273"/>
-      <c r="N5" s="271"/>
-      <c r="O5" s="272"/>
-      <c r="P5" s="272"/>
-      <c r="Q5" s="272"/>
-      <c r="R5" s="272"/>
-      <c r="S5" s="272"/>
-      <c r="T5" s="272"/>
-      <c r="U5" s="272"/>
-      <c r="V5" s="272"/>
-      <c r="W5" s="272"/>
-      <c r="X5" s="273"/>
+      <c r="A5" s="246"/>
+      <c r="B5" s="247"/>
+      <c r="C5" s="247"/>
+      <c r="D5" s="247"/>
+      <c r="E5" s="247"/>
+      <c r="F5" s="247"/>
+      <c r="G5" s="247"/>
+      <c r="H5" s="247"/>
+      <c r="I5" s="247"/>
+      <c r="J5" s="247"/>
+      <c r="K5" s="247"/>
+      <c r="L5" s="247"/>
+      <c r="M5" s="248"/>
+      <c r="N5" s="246"/>
+      <c r="O5" s="247"/>
+      <c r="P5" s="247"/>
+      <c r="Q5" s="247"/>
+      <c r="R5" s="247"/>
+      <c r="S5" s="247"/>
+      <c r="T5" s="247"/>
+      <c r="U5" s="247"/>
+      <c r="V5" s="247"/>
+      <c r="W5" s="247"/>
+      <c r="X5" s="248"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7473,66 +7479,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="248" t="s">
+      <c r="A7" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="248"/>
-      <c r="C7" s="248"/>
-      <c r="D7" s="248"/>
-      <c r="E7" s="248"/>
-      <c r="F7" s="248"/>
-      <c r="G7" s="248"/>
-      <c r="H7" s="248"/>
-      <c r="I7" s="248"/>
-      <c r="J7" s="248" t="s">
+      <c r="B7" s="245"/>
+      <c r="C7" s="245"/>
+      <c r="D7" s="245"/>
+      <c r="E7" s="245"/>
+      <c r="F7" s="245"/>
+      <c r="G7" s="245"/>
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="245" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="248"/>
-      <c r="L7" s="248"/>
-      <c r="M7" s="248"/>
-      <c r="N7" s="248"/>
-      <c r="O7" s="248"/>
-      <c r="P7" s="248" t="s">
+      <c r="K7" s="245"/>
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245"/>
+      <c r="O7" s="245"/>
+      <c r="P7" s="245" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="248"/>
-      <c r="R7" s="248"/>
-      <c r="S7" s="248"/>
-      <c r="T7" s="248"/>
-      <c r="U7" s="248"/>
-      <c r="V7" s="248"/>
-      <c r="W7" s="248"/>
-      <c r="X7" s="248"/>
+      <c r="Q7" s="245"/>
+      <c r="R7" s="245"/>
+      <c r="S7" s="245"/>
+      <c r="T7" s="245"/>
+      <c r="U7" s="245"/>
+      <c r="V7" s="245"/>
+      <c r="W7" s="245"/>
+      <c r="X7" s="245"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="254"/>
+      <c r="B8" s="254"/>
+      <c r="C8" s="254"/>
+      <c r="D8" s="254"/>
+      <c r="E8" s="254"/>
+      <c r="F8" s="254"/>
+      <c r="G8" s="254"/>
+      <c r="H8" s="254"/>
+      <c r="I8" s="254"/>
+      <c r="J8" s="255" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="256"/>
+      <c r="L8" s="256"/>
+      <c r="M8" s="256"/>
+      <c r="N8" s="256"/>
+      <c r="O8" s="257"/>
+      <c r="P8" s="255" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="256"/>
+      <c r="R8" s="256"/>
+      <c r="S8" s="256"/>
+      <c r="T8" s="256"/>
+      <c r="U8" s="256"/>
+      <c r="V8" s="256"/>
+      <c r="W8" s="256"/>
+      <c r="X8" s="257"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7561,66 +7567,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="268" t="s">
+      <c r="A10" s="258" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="268"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
-      <c r="F10" s="268"/>
-      <c r="G10" s="268"/>
-      <c r="H10" s="268"/>
-      <c r="I10" s="268"/>
-      <c r="J10" s="268"/>
-      <c r="K10" s="268"/>
-      <c r="L10" s="268"/>
-      <c r="M10" s="268"/>
-      <c r="N10" s="268"/>
-      <c r="O10" s="268"/>
-      <c r="P10" s="268"/>
-      <c r="Q10" s="268"/>
-      <c r="R10" s="268"/>
-      <c r="S10" s="268"/>
-      <c r="T10" s="268"/>
-      <c r="U10" s="268"/>
-      <c r="V10" s="268"/>
-      <c r="W10" s="268"/>
-      <c r="X10" s="268"/>
+      <c r="B10" s="258"/>
+      <c r="C10" s="258"/>
+      <c r="D10" s="258"/>
+      <c r="E10" s="258"/>
+      <c r="F10" s="258"/>
+      <c r="G10" s="258"/>
+      <c r="H10" s="258"/>
+      <c r="I10" s="258"/>
+      <c r="J10" s="258"/>
+      <c r="K10" s="258"/>
+      <c r="L10" s="258"/>
+      <c r="M10" s="258"/>
+      <c r="N10" s="258"/>
+      <c r="O10" s="258"/>
+      <c r="P10" s="258"/>
+      <c r="Q10" s="258"/>
+      <c r="R10" s="258"/>
+      <c r="S10" s="258"/>
+      <c r="T10" s="258"/>
+      <c r="U10" s="258"/>
+      <c r="V10" s="258"/>
+      <c r="W10" s="258"/>
+      <c r="X10" s="258"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="269" t="s">
+      <c r="A11" s="259" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="269"/>
-      <c r="C11" s="269"/>
-      <c r="D11" s="269"/>
-      <c r="E11" s="269"/>
-      <c r="F11" s="269"/>
-      <c r="G11" s="269" t="s">
+      <c r="B11" s="259"/>
+      <c r="C11" s="259"/>
+      <c r="D11" s="259"/>
+      <c r="E11" s="259"/>
+      <c r="F11" s="259"/>
+      <c r="G11" s="259" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="269"/>
-      <c r="I11" s="269"/>
-      <c r="J11" s="269"/>
-      <c r="K11" s="269"/>
-      <c r="L11" s="269"/>
-      <c r="M11" s="269" t="s">
+      <c r="H11" s="259"/>
+      <c r="I11" s="259"/>
+      <c r="J11" s="259"/>
+      <c r="K11" s="259"/>
+      <c r="L11" s="259"/>
+      <c r="M11" s="259" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="269"/>
-      <c r="O11" s="269"/>
-      <c r="P11" s="269"/>
-      <c r="Q11" s="269"/>
-      <c r="R11" s="269"/>
-      <c r="S11" s="269" t="s">
+      <c r="N11" s="259"/>
+      <c r="O11" s="259"/>
+      <c r="P11" s="259"/>
+      <c r="Q11" s="259"/>
+      <c r="R11" s="259"/>
+      <c r="S11" s="259" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="269"/>
-      <c r="U11" s="269"/>
-      <c r="V11" s="269"/>
-      <c r="W11" s="269"/>
-      <c r="X11" s="269"/>
+      <c r="T11" s="259"/>
+      <c r="U11" s="259"/>
+      <c r="V11" s="259"/>
+      <c r="W11" s="259"/>
+      <c r="X11" s="259"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7649,66 +7655,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="248" t="s">
+      <c r="A13" s="245" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="248"/>
-      <c r="C13" s="248"/>
-      <c r="D13" s="248"/>
-      <c r="E13" s="248"/>
-      <c r="F13" s="248"/>
-      <c r="G13" s="248"/>
-      <c r="H13" s="248"/>
-      <c r="I13" s="248"/>
-      <c r="J13" s="248" t="s">
+      <c r="B13" s="245"/>
+      <c r="C13" s="245"/>
+      <c r="D13" s="245"/>
+      <c r="E13" s="245"/>
+      <c r="F13" s="245"/>
+      <c r="G13" s="245"/>
+      <c r="H13" s="245"/>
+      <c r="I13" s="245"/>
+      <c r="J13" s="245" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="248"/>
-      <c r="L13" s="248"/>
-      <c r="M13" s="248"/>
-      <c r="N13" s="248"/>
-      <c r="O13" s="248"/>
-      <c r="P13" s="248" t="s">
+      <c r="K13" s="245"/>
+      <c r="L13" s="245"/>
+      <c r="M13" s="245"/>
+      <c r="N13" s="245"/>
+      <c r="O13" s="245"/>
+      <c r="P13" s="245" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="248"/>
-      <c r="R13" s="248"/>
-      <c r="S13" s="248"/>
-      <c r="T13" s="248"/>
-      <c r="U13" s="248"/>
-      <c r="V13" s="248"/>
-      <c r="W13" s="248"/>
-      <c r="X13" s="248"/>
+      <c r="Q13" s="245"/>
+      <c r="R13" s="245"/>
+      <c r="S13" s="245"/>
+      <c r="T13" s="245"/>
+      <c r="U13" s="245"/>
+      <c r="V13" s="245"/>
+      <c r="W13" s="245"/>
+      <c r="X13" s="245"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="254"/>
+      <c r="B14" s="254"/>
+      <c r="C14" s="254"/>
+      <c r="D14" s="254"/>
+      <c r="E14" s="254"/>
+      <c r="F14" s="254"/>
+      <c r="G14" s="254"/>
+      <c r="H14" s="254"/>
+      <c r="I14" s="254"/>
+      <c r="J14" s="255" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="256"/>
+      <c r="L14" s="256"/>
+      <c r="M14" s="256"/>
+      <c r="N14" s="256"/>
+      <c r="O14" s="257"/>
+      <c r="P14" s="255" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="256"/>
+      <c r="R14" s="256"/>
+      <c r="S14" s="256"/>
+      <c r="T14" s="256"/>
+      <c r="U14" s="256"/>
+      <c r="V14" s="256"/>
+      <c r="W14" s="256"/>
+      <c r="X14" s="257"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7737,184 +7743,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="259" t="s">
+      <c r="A16" s="265" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="259"/>
-      <c r="C16" s="259"/>
-      <c r="D16" s="259"/>
-      <c r="E16" s="259"/>
-      <c r="F16" s="259"/>
-      <c r="G16" s="259"/>
-      <c r="H16" s="259"/>
-      <c r="I16" s="259"/>
-      <c r="J16" s="260" t="s">
+      <c r="B16" s="265"/>
+      <c r="C16" s="265"/>
+      <c r="D16" s="265"/>
+      <c r="E16" s="265"/>
+      <c r="F16" s="265"/>
+      <c r="G16" s="265"/>
+      <c r="H16" s="265"/>
+      <c r="I16" s="265"/>
+      <c r="J16" s="266" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="260"/>
-      <c r="L16" s="260"/>
-      <c r="M16" s="260"/>
-      <c r="N16" s="259" t="s">
+      <c r="K16" s="266"/>
+      <c r="L16" s="266"/>
+      <c r="M16" s="266"/>
+      <c r="N16" s="265" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="259"/>
-      <c r="P16" s="259"/>
-      <c r="Q16" s="259"/>
-      <c r="R16" s="259"/>
-      <c r="S16" s="259"/>
-      <c r="T16" s="261" t="s">
+      <c r="O16" s="265"/>
+      <c r="P16" s="265"/>
+      <c r="Q16" s="265"/>
+      <c r="R16" s="265"/>
+      <c r="S16" s="265"/>
+      <c r="T16" s="267" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="261"/>
-      <c r="V16" s="261"/>
-      <c r="W16" s="261"/>
-      <c r="X16" s="261"/>
+      <c r="U16" s="267"/>
+      <c r="V16" s="267"/>
+      <c r="W16" s="267"/>
+      <c r="X16" s="267"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="249" t="s">
+      <c r="A17" s="260" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="250"/>
-      <c r="C17" s="250"/>
-      <c r="D17" s="250"/>
-      <c r="E17" s="250"/>
-      <c r="F17" s="250"/>
-      <c r="G17" s="250"/>
-      <c r="H17" s="250"/>
-      <c r="I17" s="251"/>
-      <c r="J17" s="262" t="s">
+      <c r="B17" s="252"/>
+      <c r="C17" s="252"/>
+      <c r="D17" s="252"/>
+      <c r="E17" s="252"/>
+      <c r="F17" s="252"/>
+      <c r="G17" s="252"/>
+      <c r="H17" s="252"/>
+      <c r="I17" s="261"/>
+      <c r="J17" s="268" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="263"/>
-      <c r="L17" s="263"/>
-      <c r="M17" s="264"/>
-      <c r="N17" s="249" t="s">
+      <c r="K17" s="269"/>
+      <c r="L17" s="269"/>
+      <c r="M17" s="270"/>
+      <c r="N17" s="260" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="250"/>
-      <c r="P17" s="250"/>
-      <c r="Q17" s="250"/>
-      <c r="R17" s="250"/>
-      <c r="S17" s="251"/>
-      <c r="T17" s="249" t="s">
+      <c r="O17" s="252"/>
+      <c r="P17" s="252"/>
+      <c r="Q17" s="252"/>
+      <c r="R17" s="252"/>
+      <c r="S17" s="261"/>
+      <c r="T17" s="260" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="250"/>
-      <c r="V17" s="250"/>
-      <c r="W17" s="250"/>
-      <c r="X17" s="251"/>
+      <c r="U17" s="252"/>
+      <c r="V17" s="252"/>
+      <c r="W17" s="252"/>
+      <c r="X17" s="261"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="252"/>
-      <c r="B18" s="253"/>
-      <c r="C18" s="253"/>
-      <c r="D18" s="253"/>
-      <c r="E18" s="253"/>
-      <c r="F18" s="253"/>
-      <c r="G18" s="253"/>
-      <c r="H18" s="253"/>
-      <c r="I18" s="254"/>
-      <c r="J18" s="265"/>
-      <c r="K18" s="266"/>
-      <c r="L18" s="266"/>
-      <c r="M18" s="267"/>
-      <c r="N18" s="252"/>
-      <c r="O18" s="253"/>
-      <c r="P18" s="253"/>
-      <c r="Q18" s="253"/>
-      <c r="R18" s="253"/>
-      <c r="S18" s="254"/>
-      <c r="T18" s="252"/>
-      <c r="U18" s="253"/>
-      <c r="V18" s="253"/>
-      <c r="W18" s="253"/>
-      <c r="X18" s="254"/>
+      <c r="A18" s="262"/>
+      <c r="B18" s="263"/>
+      <c r="C18" s="263"/>
+      <c r="D18" s="263"/>
+      <c r="E18" s="263"/>
+      <c r="F18" s="263"/>
+      <c r="G18" s="263"/>
+      <c r="H18" s="263"/>
+      <c r="I18" s="264"/>
+      <c r="J18" s="271"/>
+      <c r="K18" s="272"/>
+      <c r="L18" s="272"/>
+      <c r="M18" s="273"/>
+      <c r="N18" s="262"/>
+      <c r="O18" s="263"/>
+      <c r="P18" s="263"/>
+      <c r="Q18" s="263"/>
+      <c r="R18" s="263"/>
+      <c r="S18" s="264"/>
+      <c r="T18" s="262"/>
+      <c r="U18" s="263"/>
+      <c r="V18" s="263"/>
+      <c r="W18" s="263"/>
+      <c r="X18" s="264"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="247" t="s">
+      <c r="A21" s="277" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="247"/>
-      <c r="C21" s="247"/>
-      <c r="D21" s="247"/>
-      <c r="E21" s="247"/>
-      <c r="F21" s="247"/>
-      <c r="G21" s="247"/>
-      <c r="H21" s="247"/>
+      <c r="B21" s="277"/>
+      <c r="C21" s="277"/>
+      <c r="D21" s="277"/>
+      <c r="E21" s="277"/>
+      <c r="F21" s="277"/>
+      <c r="G21" s="277"/>
+      <c r="H21" s="277"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="247" t="s">
+      <c r="J21" s="277" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="247"/>
-      <c r="L21" s="247"/>
-      <c r="M21" s="247"/>
-      <c r="N21" s="247"/>
-      <c r="O21" s="247"/>
-      <c r="P21" s="247"/>
+      <c r="K21" s="277"/>
+      <c r="L21" s="277"/>
+      <c r="M21" s="277"/>
+      <c r="N21" s="277"/>
+      <c r="O21" s="277"/>
+      <c r="P21" s="277"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="247" t="s">
+      <c r="R21" s="277" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="247"/>
-      <c r="T21" s="247"/>
-      <c r="U21" s="247"/>
-      <c r="V21" s="247"/>
-      <c r="W21" s="247"/>
-      <c r="X21" s="247"/>
+      <c r="S21" s="277"/>
+      <c r="T21" s="277"/>
+      <c r="U21" s="277"/>
+      <c r="V21" s="277"/>
+      <c r="W21" s="277"/>
+      <c r="X21" s="277"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="244" t="s">
+      <c r="P23" s="274" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="244"/>
-      <c r="R23" s="244"/>
-      <c r="S23" s="244"/>
-      <c r="T23" s="244"/>
-      <c r="U23" s="245" t="s">
+      <c r="Q23" s="274"/>
+      <c r="R23" s="274"/>
+      <c r="S23" s="274"/>
+      <c r="T23" s="274"/>
+      <c r="U23" s="275" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="245"/>
-      <c r="W23" s="245"/>
-      <c r="X23" s="245"/>
+      <c r="V23" s="275"/>
+      <c r="W23" s="275"/>
+      <c r="X23" s="275"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="244" t="s">
+      <c r="P24" s="274" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="244"/>
-      <c r="R24" s="244"/>
-      <c r="S24" s="244"/>
-      <c r="T24" s="244"/>
-      <c r="U24" s="246" t="s">
+      <c r="Q24" s="274"/>
+      <c r="R24" s="274"/>
+      <c r="S24" s="274"/>
+      <c r="T24" s="274"/>
+      <c r="U24" s="276" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="246"/>
-      <c r="W24" s="246"/>
-      <c r="X24" s="246"/>
+      <c r="V24" s="276"/>
+      <c r="W24" s="276"/>
+      <c r="X24" s="276"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7929,13 +7923,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
varibles css / mejora al aplicar el xml en blogger
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva - copia.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6411244E-23B7-4993-B6F6-5AE656DEE7C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55540C8A-BF86-4084-BA05-D1953070C29D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,33 +25,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>SENA CAT</author>
-  </authors>
-  <commentList>
-    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{96982A9A-617F-4D05-B03B-BA3B0D8F3069}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{7D603635-B1DF-4C5D-8B0E-F4A234119AF6}">
-      <text/>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -901,16 +874,6 @@
     <t>SI</t>
   </si>
   <si>
-    <t>Decoré el botón de descarga para que se viera más estético, además de arreglar un bug que hacía que se insertara fuera de su contenedor padre.
-Después de esto, decidí dedicar el resto del día a cambiar la visualización de las imágenes solo con JS. Estuve todo el día en eso, pero tuve muchos problemas de visualización, rendimiento, responsividad y compatibilidad con los botones de descarga. Viendo todo esto, decidí archivar el código y no continuar desarrollándolo, ya que no valía la pena todo el tiempo invertido en algo que probablemente afectaría el rendimiento.
-Supongo que algo positivo de todo esto es que el código del carrusel original ahora admite más de un carrusel en la misma página, lo cual está bastante bien por si necesito otro en el futuro.</t>
-  </si>
-  <si>
-    <t>Definitivamente, no poder modificar el código del cuerpo de los posts directamente me fastidió la tarde. Si pudiera modificar el HTML, podría haber hecho esto de una forma fácil.
-Leí la documentación y, desafortunadamente, no encontré información sobre esto. La verdad, creo que debería dejar de intentar modificar más el post-body para no perder el tiempo como lo hice hoy.
-Aunque aún hay cosas que quiero cambiar de él.</t>
-  </si>
-  <si>
     <t>Mejoré la visualización de múltiples imágenes desde el escritorio: ahora son más pequeñas y, cuando hay dos o un sobrante en la siguiente fila, estas aumentan su tamaño para ocupar tres hileras, evitando que la tarjeta se vea vacía.
 Cuando hay una o dos imágenes en pantalla, conservan su tamaño grande para un mejor aspecto.
 Hice que el carrusel de imágenes solo se vea en la página principal y no en las demás.
@@ -1006,12 +969,20 @@
 combine la función de agregar botones y la de agregar la biblioteca de visualización de imágenes, ademas puse variables globales a las cosas relacionadas con posts 
  encontré la forma de desactivar el visor de imágenes por defecto de Blogger y lo inclui a la documentacion</t>
   </si>
+  <si>
+    <t>cree compatibilidad para poder agregarlo a un blogger totalmente nuevo, ademas de esto agregre en el README configuraciones que se tienen que hacer desde blogger antes de aplicar la plantilla
+cambie de posicion los estilos del menu, ya que descubri que en la posicion que estaban hacia que los mismo no se aplicaran inmediatamente probocando errores visuales
+comenze a trabajar con variables en el css para poder cambiarlas facilmente desde el editor de blogger (esto para que sea personalizable por los que manejen el blog)</t>
+  </si>
+  <si>
+    <t>falle muchas veces intentando ver la forma en que poder agregar secciones y variables compatibles con el editor de blogger</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1273,12 +1244,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -2863,6 +2828,42 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="82" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2875,6 +2876,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2926,77 +2966,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3016,99 +3071,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3127,86 +3170,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4193,56 +4158,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="170"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="172"/>
-      <c r="D4" s="172"/>
-      <c r="E4" s="173"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="174" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="175"/>
-      <c r="D5" s="175"/>
-      <c r="E5" s="176"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="173"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="168" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="170"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4254,29 +4219,29 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="177" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="178"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="179" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="180"/>
-      <c r="E9" s="181"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="182" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="183"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="184"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="185" t="s">
@@ -4287,12 +4252,12 @@
       <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="164" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="165"/>
-      <c r="D12" s="166"/>
-      <c r="E12" s="167"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4303,68 +4268,68 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="197" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="198"/>
-      <c r="D14" s="198"/>
-      <c r="E14" s="199"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="200" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="201"/>
-      <c r="D15" s="201"/>
-      <c r="E15" s="202"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="200" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="201"/>
-      <c r="D16" s="201"/>
-      <c r="E16" s="202"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="206" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="207"/>
-      <c r="D17" s="207"/>
-      <c r="E17" s="208"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="200" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="201"/>
-      <c r="D18" s="201"/>
-      <c r="E18" s="202"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="200" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="201"/>
-      <c r="D19" s="201"/>
-      <c r="E19" s="202"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="203" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="204"/>
-      <c r="D20" s="204"/>
-      <c r="E20" s="205"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="164" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="165"/>
-      <c r="D21" s="166"/>
-      <c r="E21" s="167"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="185" t="s">
@@ -4402,8 +4367,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="193"/>
-      <c r="E25" s="194"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4412,8 +4377,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="193"/>
-      <c r="E26" s="194"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4422,8 +4387,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="193"/>
-      <c r="E27" s="194"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4432,8 +4397,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="193"/>
-      <c r="E28" s="194"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4442,10 +4407,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="193" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="194" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4456,10 +4421,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="193" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="194" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4470,8 +4435,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="193"/>
-      <c r="E31" s="194"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4480,10 +4445,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="193" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="194" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4494,8 +4459,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="193"/>
-      <c r="E33" s="194"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4504,8 +4469,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="193"/>
-      <c r="E34" s="194"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4514,8 +4479,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="193"/>
-      <c r="E35" s="194"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4524,8 +4489,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="193"/>
-      <c r="E36" s="194"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4534,8 +4499,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="193"/>
-      <c r="E37" s="194"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4544,8 +4509,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="193"/>
-      <c r="E38" s="194"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4554,8 +4519,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="193"/>
-      <c r="E39" s="194"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4564,8 +4529,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="193"/>
-      <c r="E40" s="194"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4574,8 +4539,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="193"/>
-      <c r="E41" s="194"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4584,8 +4549,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="193"/>
-      <c r="E42" s="194"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4594,10 +4559,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="193" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="194" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4608,8 +4573,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="193"/>
-      <c r="E44" s="194"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4618,8 +4583,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="193"/>
-      <c r="E45" s="194"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4628,8 +4593,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="193"/>
-      <c r="E46" s="194"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4638,10 +4603,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="193" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="194" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4652,8 +4617,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="193"/>
-      <c r="E48" s="194"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4662,10 +4627,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="193" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="194" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4676,10 +4641,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="193" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="194" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4690,10 +4655,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="193" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="194" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4704,8 +4669,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="193"/>
-      <c r="E52" s="194"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4714,8 +4679,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="193"/>
-      <c r="E53" s="194"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4724,8 +4689,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="193"/>
-      <c r="E54" s="194"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4734,8 +4699,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="193"/>
-      <c r="E55" s="194"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4744,8 +4709,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="193"/>
-      <c r="E56" s="194"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4754,10 +4719,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="195" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="196" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4775,6 +4740,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4791,44 +4794,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4837,14 +4802,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74A078B-FDD5-4F89-B4CB-7471575D0D0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74A078B-FDD5-4F89-B4CB-7471575D0D0F}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4926,14 +4891,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="170"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4955,14 +4920,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="172"/>
-      <c r="D4" s="172"/>
-      <c r="E4" s="172"/>
-      <c r="F4" s="172"/>
-      <c r="G4" s="173"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4984,14 +4949,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="168" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -5013,14 +4978,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="172"/>
-      <c r="F6" s="172"/>
-      <c r="G6" s="173"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -5042,14 +5007,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="168" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5245,16 +5210,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="215">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="220"/>
-      <c r="D14" s="216"/>
-      <c r="E14" s="217" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="218"/>
-      <c r="G14" s="219"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5326,20 +5291,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="215" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="216"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>6</v>
       </c>
-      <c r="F17" s="221" t="s">
+      <c r="F17" s="228" t="s">
         <v>200</v>
       </c>
-      <c r="G17" s="222"/>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5407,20 +5372,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="215" t="s">
+      <c r="B20" s="223" t="s">
         <v>203</v>
       </c>
-      <c r="C20" s="216"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>201</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="241" t="s">
+      <c r="F20" s="237" t="s">
         <v>202</v>
       </c>
-      <c r="G20" s="242"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5462,14 +5427,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="212" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="213"/>
-      <c r="D22" s="213"/>
-      <c r="E22" s="213"/>
-      <c r="F22" s="213"/>
-      <c r="G22" s="214"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5494,17 +5459,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="240" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="216"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="241" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="242"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5648,10 +5613,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="209" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="210"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5678,8 +5643,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="209"/>
-      <c r="G29" s="210"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -6017,10 +5982,10 @@
       <c r="Y39" s="18"/>
     </row>
     <row r="40" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="235" t="s">
-        <v>224</v>
-      </c>
-      <c r="C40" s="236"/>
+      <c r="B40" s="216" t="s">
+        <v>222</v>
+      </c>
+      <c r="C40" s="217"/>
       <c r="D40" s="161">
         <v>45735</v>
       </c>
@@ -6031,7 +5996,7 @@
         <v>205</v>
       </c>
       <c r="G40" s="160" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
@@ -6053,10 +6018,10 @@
       <c r="Y40" s="18"/>
     </row>
     <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="235" t="s">
-        <v>227</v>
-      </c>
-      <c r="C41" s="236"/>
+      <c r="B41" s="216" t="s">
+        <v>225</v>
+      </c>
+      <c r="C41" s="217"/>
       <c r="D41" s="161">
         <v>45736</v>
       </c>
@@ -6067,7 +6032,7 @@
         <v>205</v>
       </c>
       <c r="G41" s="160" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
@@ -6089,21 +6054,21 @@
       <c r="Y41" s="18"/>
     </row>
     <row r="42" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="235" t="s">
-        <v>207</v>
-      </c>
-      <c r="C42" s="236"/>
+      <c r="B42" s="216" t="s">
+        <v>226</v>
+      </c>
+      <c r="C42" s="217"/>
       <c r="D42" s="161">
-        <v>45722</v>
+        <v>45737</v>
       </c>
       <c r="E42" s="161">
-        <v>45722</v>
+        <v>45737</v>
       </c>
       <c r="F42" s="160" t="s">
         <v>205</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6125,10 +6090,10 @@
       <c r="Y42" s="18"/>
     </row>
     <row r="43" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="235" t="s">
-        <v>209</v>
-      </c>
-      <c r="C43" s="236"/>
+      <c r="B43" s="216" t="s">
+        <v>207</v>
+      </c>
+      <c r="C43" s="217"/>
       <c r="D43" s="161">
         <v>45723</v>
       </c>
@@ -6139,7 +6104,7 @@
         <v>205</v>
       </c>
       <c r="G43" s="160" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H43" s="20"/>
       <c r="I43" s="18"/>
@@ -6161,8 +6126,8 @@
       <c r="Y43" s="18"/>
     </row>
     <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="235"/>
-      <c r="C44" s="236"/>
+      <c r="B44" s="216"/>
+      <c r="C44" s="217"/>
       <c r="D44" s="161"/>
       <c r="E44" s="161"/>
       <c r="F44" s="160"/>
@@ -6187,8 +6152,8 @@
       <c r="Y44" s="18"/>
     </row>
     <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="235"/>
-      <c r="C45" s="236"/>
+      <c r="B45" s="216"/>
+      <c r="C45" s="217"/>
       <c r="D45" s="161"/>
       <c r="E45" s="161"/>
       <c r="F45" s="160"/>
@@ -6213,10 +6178,10 @@
       <c r="Y45" s="18"/>
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="235" t="s">
-        <v>211</v>
-      </c>
-      <c r="C46" s="236"/>
+      <c r="B46" s="216" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" s="217"/>
       <c r="D46" s="161">
         <v>45726</v>
       </c>
@@ -6227,7 +6192,7 @@
         <v>205</v>
       </c>
       <c r="G46" s="160" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="18"/>
@@ -6249,10 +6214,10 @@
       <c r="Y46" s="18"/>
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="235" t="s">
-        <v>213</v>
-      </c>
-      <c r="C47" s="236"/>
+      <c r="B47" s="216" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" s="217"/>
       <c r="D47" s="161">
         <v>45727</v>
       </c>
@@ -6263,7 +6228,7 @@
         <v>205</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6285,10 +6250,10 @@
       <c r="Y47" s="18"/>
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="235" t="s">
-        <v>217</v>
-      </c>
-      <c r="C48" s="236"/>
+      <c r="B48" s="216" t="s">
+        <v>215</v>
+      </c>
+      <c r="C48" s="217"/>
       <c r="D48" s="161">
         <v>45728</v>
       </c>
@@ -6299,7 +6264,7 @@
         <v>205</v>
       </c>
       <c r="G48" s="160" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
@@ -6321,10 +6286,10 @@
       <c r="Y48" s="18"/>
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="235" t="s">
-        <v>215</v>
-      </c>
-      <c r="C49" s="236"/>
+      <c r="B49" s="216" t="s">
+        <v>213</v>
+      </c>
+      <c r="C49" s="217"/>
       <c r="D49" s="161">
         <v>45729</v>
       </c>
@@ -6335,7 +6300,7 @@
         <v>205</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6357,10 +6322,10 @@
       <c r="Y49" s="18"/>
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="235" t="s">
-        <v>219</v>
-      </c>
-      <c r="C50" s="236"/>
+      <c r="B50" s="216" t="s">
+        <v>217</v>
+      </c>
+      <c r="C50" s="217"/>
       <c r="D50" s="161">
         <v>45730</v>
       </c>
@@ -6371,7 +6336,7 @@
         <v>205</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6393,8 +6358,8 @@
       <c r="Y50" s="18"/>
     </row>
     <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="235"/>
-      <c r="C51" s="236"/>
+      <c r="B51" s="216"/>
+      <c r="C51" s="217"/>
       <c r="D51" s="161"/>
       <c r="E51" s="161"/>
       <c r="F51" s="160"/>
@@ -6419,8 +6384,8 @@
       <c r="Y51" s="18"/>
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="235"/>
-      <c r="C52" s="236"/>
+      <c r="B52" s="216"/>
+      <c r="C52" s="217"/>
       <c r="D52" s="161"/>
       <c r="E52" s="161"/>
       <c r="F52" s="160"/>
@@ -6445,10 +6410,10 @@
       <c r="Y52" s="18"/>
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="235" t="s">
-        <v>221</v>
-      </c>
-      <c r="C53" s="236"/>
+      <c r="B53" s="216" t="s">
+        <v>219</v>
+      </c>
+      <c r="C53" s="217"/>
       <c r="D53" s="161">
         <v>45733</v>
       </c>
@@ -6459,7 +6424,7 @@
         <v>205</v>
       </c>
       <c r="G53" s="160" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H53" s="20"/>
       <c r="I53" s="18"/>
@@ -6481,10 +6446,10 @@
       <c r="Y53" s="18"/>
     </row>
     <row r="54" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="235" t="s">
-        <v>223</v>
-      </c>
-      <c r="C54" s="236"/>
+      <c r="B54" s="216" t="s">
+        <v>221</v>
+      </c>
+      <c r="C54" s="217"/>
       <c r="D54" s="161">
         <v>45734</v>
       </c>
@@ -6514,7 +6479,7 @@
     </row>
     <row r="55" spans="2:26" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="27"/>
-      <c r="C55" s="278"/>
+      <c r="C55" s="164"/>
       <c r="D55" s="20"/>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
@@ -6567,14 +6532,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="237" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="238"/>
-      <c r="D57" s="238"/>
-      <c r="E57" s="238"/>
-      <c r="F57" s="238"/>
-      <c r="G57" s="239"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6833,9 +6798,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="225"/>
-      <c r="C66" s="225"/>
-      <c r="D66" s="225"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6860,11 +6825,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="225"/>
-      <c r="C67" s="225"/>
-      <c r="D67" s="225"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="227" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6889,10 +6854,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="226"/>
-      <c r="C68" s="226"/>
-      <c r="D68" s="226"/>
-      <c r="F68" s="228"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6915,11 +6880,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="211" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="211"/>
-      <c r="D69" s="211"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6971,11 +6936,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="223"/>
-      <c r="C71" s="223"/>
-      <c r="D71" s="223"/>
-      <c r="F71" s="243"/>
-      <c r="G71" s="243"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6997,11 +6962,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="224"/>
-      <c r="C72" s="224"/>
-      <c r="D72" s="224"/>
-      <c r="F72" s="218"/>
-      <c r="G72" s="218"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -7028,10 +6993,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="211" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="211"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7109,14 +7074,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="229" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="230"/>
-      <c r="D76" s="230"/>
-      <c r="E76" s="230"/>
-      <c r="F76" s="230"/>
-      <c r="G76" s="231"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7138,14 +7103,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="232" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="233"/>
-      <c r="D77" s="233"/>
-      <c r="E77" s="233"/>
-      <c r="F77" s="233"/>
-      <c r="G77" s="234"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7176,14 +7141,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7200,22 +7173,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7226,7 +7191,6 @@
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="47" fitToHeight="0" orientation="portrait" horizontalDpi="4294967294" r:id="rId5"/>
   <drawing r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -7333,124 +7297,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="244" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="244"/>
-      <c r="C1" s="244"/>
-      <c r="D1" s="244"/>
-      <c r="E1" s="244"/>
-      <c r="F1" s="244"/>
-      <c r="G1" s="244"/>
-      <c r="H1" s="244"/>
-      <c r="I1" s="244"/>
-      <c r="J1" s="244"/>
-      <c r="K1" s="244"/>
-      <c r="L1" s="244"/>
-      <c r="M1" s="244"/>
-      <c r="N1" s="244"/>
-      <c r="O1" s="244"/>
-      <c r="P1" s="244"/>
-      <c r="Q1" s="244"/>
-      <c r="R1" s="244"/>
-      <c r="S1" s="244"/>
-      <c r="T1" s="244"/>
-      <c r="U1" s="244" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="244"/>
-      <c r="W1" s="244"/>
-      <c r="X1" s="244"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="244"/>
-      <c r="B2" s="244"/>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
-      <c r="M2" s="244"/>
-      <c r="N2" s="244"/>
-      <c r="O2" s="244"/>
-      <c r="P2" s="244"/>
-      <c r="Q2" s="244"/>
-      <c r="R2" s="244"/>
-      <c r="S2" s="244"/>
-      <c r="T2" s="244"/>
-      <c r="U2" s="252" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="252"/>
-      <c r="W2" s="252"/>
-      <c r="X2" s="252"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="253"/>
-      <c r="V3" s="253"/>
-      <c r="W3" s="253"/>
-      <c r="X3" s="253"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="249" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="250"/>
-      <c r="C4" s="250"/>
-      <c r="D4" s="250"/>
-      <c r="E4" s="250"/>
-      <c r="F4" s="250"/>
-      <c r="G4" s="250"/>
-      <c r="H4" s="250"/>
-      <c r="I4" s="250"/>
-      <c r="J4" s="250"/>
-      <c r="K4" s="250"/>
-      <c r="L4" s="250"/>
-      <c r="M4" s="251"/>
-      <c r="N4" s="249" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="250"/>
-      <c r="P4" s="250"/>
-      <c r="Q4" s="250"/>
-      <c r="R4" s="250"/>
-      <c r="S4" s="250"/>
-      <c r="T4" s="250"/>
-      <c r="U4" s="250"/>
-      <c r="V4" s="250"/>
-      <c r="W4" s="250"/>
-      <c r="X4" s="251"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="246"/>
-      <c r="B5" s="247"/>
-      <c r="C5" s="247"/>
-      <c r="D5" s="247"/>
-      <c r="E5" s="247"/>
-      <c r="F5" s="247"/>
-      <c r="G5" s="247"/>
-      <c r="H5" s="247"/>
-      <c r="I5" s="247"/>
-      <c r="J5" s="247"/>
-      <c r="K5" s="247"/>
-      <c r="L5" s="247"/>
-      <c r="M5" s="248"/>
-      <c r="N5" s="246"/>
-      <c r="O5" s="247"/>
-      <c r="P5" s="247"/>
-      <c r="Q5" s="247"/>
-      <c r="R5" s="247"/>
-      <c r="S5" s="247"/>
-      <c r="T5" s="247"/>
-      <c r="U5" s="247"/>
-      <c r="V5" s="247"/>
-      <c r="W5" s="247"/>
-      <c r="X5" s="248"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7479,66 +7443,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="245" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="245"/>
-      <c r="C7" s="245"/>
-      <c r="D7" s="245"/>
-      <c r="E7" s="245"/>
-      <c r="F7" s="245"/>
-      <c r="G7" s="245"/>
-      <c r="H7" s="245"/>
-      <c r="I7" s="245"/>
-      <c r="J7" s="245" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="245"/>
-      <c r="L7" s="245"/>
-      <c r="M7" s="245"/>
-      <c r="N7" s="245"/>
-      <c r="O7" s="245"/>
-      <c r="P7" s="245" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="245"/>
-      <c r="R7" s="245"/>
-      <c r="S7" s="245"/>
-      <c r="T7" s="245"/>
-      <c r="U7" s="245"/>
-      <c r="V7" s="245"/>
-      <c r="W7" s="245"/>
-      <c r="X7" s="245"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="254"/>
-      <c r="B8" s="254"/>
-      <c r="C8" s="254"/>
-      <c r="D8" s="254"/>
-      <c r="E8" s="254"/>
-      <c r="F8" s="254"/>
-      <c r="G8" s="254"/>
-      <c r="H8" s="254"/>
-      <c r="I8" s="254"/>
-      <c r="J8" s="255" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="256"/>
-      <c r="L8" s="256"/>
-      <c r="M8" s="256"/>
-      <c r="N8" s="256"/>
-      <c r="O8" s="257"/>
-      <c r="P8" s="255" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="256"/>
-      <c r="R8" s="256"/>
-      <c r="S8" s="256"/>
-      <c r="T8" s="256"/>
-      <c r="U8" s="256"/>
-      <c r="V8" s="256"/>
-      <c r="W8" s="256"/>
-      <c r="X8" s="257"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7567,66 +7531,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="258" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="258"/>
-      <c r="C10" s="258"/>
-      <c r="D10" s="258"/>
-      <c r="E10" s="258"/>
-      <c r="F10" s="258"/>
-      <c r="G10" s="258"/>
-      <c r="H10" s="258"/>
-      <c r="I10" s="258"/>
-      <c r="J10" s="258"/>
-      <c r="K10" s="258"/>
-      <c r="L10" s="258"/>
-      <c r="M10" s="258"/>
-      <c r="N10" s="258"/>
-      <c r="O10" s="258"/>
-      <c r="P10" s="258"/>
-      <c r="Q10" s="258"/>
-      <c r="R10" s="258"/>
-      <c r="S10" s="258"/>
-      <c r="T10" s="258"/>
-      <c r="U10" s="258"/>
-      <c r="V10" s="258"/>
-      <c r="W10" s="258"/>
-      <c r="X10" s="258"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="259" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="259"/>
-      <c r="C11" s="259"/>
-      <c r="D11" s="259"/>
-      <c r="E11" s="259"/>
-      <c r="F11" s="259"/>
-      <c r="G11" s="259" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="259"/>
-      <c r="I11" s="259"/>
-      <c r="J11" s="259"/>
-      <c r="K11" s="259"/>
-      <c r="L11" s="259"/>
-      <c r="M11" s="259" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="259"/>
-      <c r="O11" s="259"/>
-      <c r="P11" s="259"/>
-      <c r="Q11" s="259"/>
-      <c r="R11" s="259"/>
-      <c r="S11" s="259" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="259"/>
-      <c r="U11" s="259"/>
-      <c r="V11" s="259"/>
-      <c r="W11" s="259"/>
-      <c r="X11" s="259"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7655,66 +7619,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="245" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="245"/>
-      <c r="C13" s="245"/>
-      <c r="D13" s="245"/>
-      <c r="E13" s="245"/>
-      <c r="F13" s="245"/>
-      <c r="G13" s="245"/>
-      <c r="H13" s="245"/>
-      <c r="I13" s="245"/>
-      <c r="J13" s="245" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="245"/>
-      <c r="L13" s="245"/>
-      <c r="M13" s="245"/>
-      <c r="N13" s="245"/>
-      <c r="O13" s="245"/>
-      <c r="P13" s="245" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="245"/>
-      <c r="R13" s="245"/>
-      <c r="S13" s="245"/>
-      <c r="T13" s="245"/>
-      <c r="U13" s="245"/>
-      <c r="V13" s="245"/>
-      <c r="W13" s="245"/>
-      <c r="X13" s="245"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="254"/>
-      <c r="B14" s="254"/>
-      <c r="C14" s="254"/>
-      <c r="D14" s="254"/>
-      <c r="E14" s="254"/>
-      <c r="F14" s="254"/>
-      <c r="G14" s="254"/>
-      <c r="H14" s="254"/>
-      <c r="I14" s="254"/>
-      <c r="J14" s="255" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="256"/>
-      <c r="L14" s="256"/>
-      <c r="M14" s="256"/>
-      <c r="N14" s="256"/>
-      <c r="O14" s="257"/>
-      <c r="P14" s="255" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="256"/>
-      <c r="R14" s="256"/>
-      <c r="S14" s="256"/>
-      <c r="T14" s="256"/>
-      <c r="U14" s="256"/>
-      <c r="V14" s="256"/>
-      <c r="W14" s="256"/>
-      <c r="X14" s="257"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7743,172 +7707,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="265" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="265"/>
-      <c r="C16" s="265"/>
-      <c r="D16" s="265"/>
-      <c r="E16" s="265"/>
-      <c r="F16" s="265"/>
-      <c r="G16" s="265"/>
-      <c r="H16" s="265"/>
-      <c r="I16" s="265"/>
-      <c r="J16" s="266" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="266"/>
-      <c r="L16" s="266"/>
-      <c r="M16" s="266"/>
-      <c r="N16" s="265" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="265"/>
-      <c r="P16" s="265"/>
-      <c r="Q16" s="265"/>
-      <c r="R16" s="265"/>
-      <c r="S16" s="265"/>
-      <c r="T16" s="267" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="267"/>
-      <c r="V16" s="267"/>
-      <c r="W16" s="267"/>
-      <c r="X16" s="267"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="260" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="252"/>
-      <c r="C17" s="252"/>
-      <c r="D17" s="252"/>
-      <c r="E17" s="252"/>
-      <c r="F17" s="252"/>
-      <c r="G17" s="252"/>
-      <c r="H17" s="252"/>
-      <c r="I17" s="261"/>
-      <c r="J17" s="268" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="269"/>
-      <c r="L17" s="269"/>
-      <c r="M17" s="270"/>
-      <c r="N17" s="260" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="252"/>
-      <c r="P17" s="252"/>
-      <c r="Q17" s="252"/>
-      <c r="R17" s="252"/>
-      <c r="S17" s="261"/>
-      <c r="T17" s="260" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="252"/>
-      <c r="V17" s="252"/>
-      <c r="W17" s="252"/>
-      <c r="X17" s="261"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="262"/>
-      <c r="B18" s="263"/>
-      <c r="C18" s="263"/>
-      <c r="D18" s="263"/>
-      <c r="E18" s="263"/>
-      <c r="F18" s="263"/>
-      <c r="G18" s="263"/>
-      <c r="H18" s="263"/>
-      <c r="I18" s="264"/>
-      <c r="J18" s="271"/>
-      <c r="K18" s="272"/>
-      <c r="L18" s="272"/>
-      <c r="M18" s="273"/>
-      <c r="N18" s="262"/>
-      <c r="O18" s="263"/>
-      <c r="P18" s="263"/>
-      <c r="Q18" s="263"/>
-      <c r="R18" s="263"/>
-      <c r="S18" s="264"/>
-      <c r="T18" s="262"/>
-      <c r="U18" s="263"/>
-      <c r="V18" s="263"/>
-      <c r="W18" s="263"/>
-      <c r="X18" s="264"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="277" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="277"/>
-      <c r="C21" s="277"/>
-      <c r="D21" s="277"/>
-      <c r="E21" s="277"/>
-      <c r="F21" s="277"/>
-      <c r="G21" s="277"/>
-      <c r="H21" s="277"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="277" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="277"/>
-      <c r="L21" s="277"/>
-      <c r="M21" s="277"/>
-      <c r="N21" s="277"/>
-      <c r="O21" s="277"/>
-      <c r="P21" s="277"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="277" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="277"/>
-      <c r="T21" s="277"/>
-      <c r="U21" s="277"/>
-      <c r="V21" s="277"/>
-      <c r="W21" s="277"/>
-      <c r="X21" s="277"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="274" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="274"/>
-      <c r="R23" s="274"/>
-      <c r="S23" s="274"/>
-      <c r="T23" s="274"/>
-      <c r="U23" s="275" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="275"/>
-      <c r="W23" s="275"/>
-      <c r="X23" s="275"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="274" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="274"/>
-      <c r="R24" s="274"/>
-      <c r="S24" s="274"/>
-      <c r="T24" s="274"/>
-      <c r="U24" s="276" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="276"/>
-      <c r="W24" s="276"/>
-      <c r="X24" s="276"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7923,25 +7899,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
reorganizacion en el editor de blogger
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva - copia.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E395BC7-70DC-445A-9D1F-5F83CBF96C49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA9B6F2-AC3F-426D-99A5-FA3E2D699289}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -885,16 +885,6 @@
     <t>Bueno, además de esto, quería entender cómo funcionaban las secciones para agregar nuevas, pero me dio muchos problemas y, al final, decidí mejor seguir moviendo cosas.</t>
   </si>
   <si>
-    <t xml:space="preserve">Hoy me dediqué a mejorar la documentación que tenía. Ahora está toda organizada en un archivo README.txt, siguiendo las pautas de GitHub. Como se puede ver en la imagen, aunque es un documento de solo texto, gracias a comandos y símbolos se puede hacer que sea más agradable a la vista. También incluí enlaces a la documentación de Blogger.
-Adicionalmente, hice cambios al protector de pantalla. Su diseño ha cambiado y ahora, cuando se toca fuera del iframe, el protector vuelve a aparecer. Esto también es compatible con el touch en dispositivos móviles.
-Además, optimicé el código de la inserción de "posts de X", logrando que se renderice un poco más rápido. Ahora tiene un mini scroll en móviles, aunque estoy considerando removerlo en la versión de PC.
-</t>
-  </si>
-  <si>
-    <t>De nuevo, cada vez noto que estoy dejando más código suelto. Es difícil ubicarme e incluso me pierdo a veces.
-Sinceramente, debo priorizar más esto, o va a convertirse en un efecto bola de nieve, aumentando la dificultad de las nuevas implementaciones.</t>
-  </si>
-  <si>
     <t>Investigué más sobre las secciones y también creé algunos archivos XML desde cero para entender cómo funcionaban. Ya logré agregarlas, aunque aún me falta encontrar la forma de posicionarlas correctamente.
 Creé el header vinculado a una de estas nuevas secciones. Es editable y lo hice a partir de un widget por defecto de Blogger. Reescribí su código y lo optimicé para que fuera más comprensible y compatible con todo tipo de tamaños de imágenes.
 Ahora mismo necesito la ayuda de alguien de medios audiovisuales para crear una imagen de 1280 x 200 para el blog. Aunque el título y la descripción son totalmente personalizables y se pueden ocultar desde la interfaz de Blogger.</t>
@@ -957,6 +947,12 @@
   </si>
   <si>
     <t>buscar la forma en quitar el flex de blogger pero mantenerlo en la pagina wep</t>
+  </si>
+  <si>
+    <t>resolvi el bug que hacia tener una mala vizualizacion del menu lateral en el editor de blogger, acomode los modulos de forma mas intuitiva, cambie la forma en que se organizan las secciones dentro del main, algo mas intuitivo y previene temblores en el diseño</t>
+  </si>
+  <si>
+    <t>resolver los problema del editor de blogger me tomo mucho, tuve que ver como funcionaban y despues de prueba y error acomode el codigo en parte donde blogger no leyera el display flex, y tambien demore mucho en descubrir como poner dos secciones en la misma fila como lo hise con la seccion principal y lateral en el editor</t>
   </si>
 </sst>
 </file>
@@ -2812,6 +2808,99 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2845,18 +2934,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2866,85 +2943,79 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2965,12 +3036,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2983,74 +3048,95 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3063,96 +3149,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4139,56 +4135,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="201"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4200,45 +4196,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="202" t="s">
+      <c r="D8" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="179"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="204" t="s">
+      <c r="B9" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="206"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="208"/>
-      <c r="E10" s="209"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="185"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="186"/>
-      <c r="D11" s="186"/>
-      <c r="E11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="188"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="179"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4249,84 +4245,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="200"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="202"/>
+      <c r="E16" s="203"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="180" t="s">
+      <c r="B17" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="181"/>
-      <c r="D17" s="181"/>
-      <c r="E17" s="182"/>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="209"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="203"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="170" t="s">
+      <c r="B19" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="203"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="175"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="206"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="186"/>
-      <c r="D22" s="186" t="s">
+      <c r="C22" s="187"/>
+      <c r="D22" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="187"/>
+      <c r="E22" s="188"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="188"/>
-      <c r="C23" s="189"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="190"/>
+      <c r="B23" s="189"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4335,10 +4331,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="192"/>
+      <c r="E24" s="193"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4348,8 +4344,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="183"/>
-      <c r="E25" s="184"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4358,8 +4354,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="183"/>
-      <c r="E26" s="184"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="195"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4368,8 +4364,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="183"/>
-      <c r="E27" s="184"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="195"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4378,8 +4374,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4388,10 +4384,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="183" t="s">
+      <c r="D29" s="194" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="184" t="s">
+      <c r="E29" s="195" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4402,10 +4398,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="195" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4416,8 +4412,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="194"/>
+      <c r="E31" s="195"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4426,10 +4422,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="184" t="s">
+      <c r="E32" s="195" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4440,8 +4436,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4450,8 +4446,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="195"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4460,8 +4456,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="194"/>
+      <c r="E35" s="195"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4470,8 +4466,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="194"/>
+      <c r="E36" s="195"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4480,8 +4476,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="195"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4490,8 +4486,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="195"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4500,8 +4496,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4510,8 +4506,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="195"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4520,8 +4516,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="195"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4530,8 +4526,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="194"/>
+      <c r="E42" s="195"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4540,10 +4536,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="183" t="s">
+      <c r="D43" s="194" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="184" t="s">
+      <c r="E43" s="195" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4554,8 +4550,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="195"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4564,8 +4560,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="194"/>
+      <c r="E45" s="195"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4574,8 +4570,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4584,10 +4580,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="183" t="s">
+      <c r="D47" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="184" t="s">
+      <c r="E47" s="195" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4598,8 +4594,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="183"/>
-      <c r="E48" s="184"/>
+      <c r="D48" s="194"/>
+      <c r="E48" s="195"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4608,10 +4604,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="183" t="s">
+      <c r="D49" s="194" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="184" t="s">
+      <c r="E49" s="195" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4622,10 +4618,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="183" t="s">
+      <c r="D50" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="184" t="s">
+      <c r="E50" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4636,10 +4632,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="183" t="s">
+      <c r="D51" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="184" t="s">
+      <c r="E51" s="195" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4650,8 +4646,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="183"/>
-      <c r="E52" s="184"/>
+      <c r="D52" s="194"/>
+      <c r="E52" s="195"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4660,8 +4656,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="183"/>
-      <c r="E53" s="184"/>
+      <c r="D53" s="194"/>
+      <c r="E53" s="195"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4670,8 +4666,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="183"/>
-      <c r="E54" s="184"/>
+      <c r="D54" s="194"/>
+      <c r="E54" s="195"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4680,8 +4676,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="183"/>
-      <c r="E55" s="184"/>
+      <c r="D55" s="194"/>
+      <c r="E55" s="195"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4690,8 +4686,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="183"/>
-      <c r="E56" s="184"/>
+      <c r="D56" s="194"/>
+      <c r="E56" s="195"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4700,10 +4696,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="165" t="s">
+      <c r="D57" s="196" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="197" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4721,44 +4717,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4775,6 +4733,44 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4789,8 +4785,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4872,14 +4868,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4901,14 +4897,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="198"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="174"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4930,14 +4926,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="194"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="194"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4959,14 +4955,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="174"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4988,14 +4984,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="194"/>
-      <c r="D7" s="194"/>
-      <c r="E7" s="194"/>
-      <c r="F7" s="194"/>
-      <c r="G7" s="195"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5191,16 +5187,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="223">
+      <c r="B14" s="218">
         <v>2557356</v>
       </c>
-      <c r="C14" s="227"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="225" t="s">
+      <c r="C14" s="223"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="220" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="222"/>
-      <c r="G14" s="226"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="222"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5272,20 +5268,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="224"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>6</v>
       </c>
-      <c r="F17" s="228" t="s">
+      <c r="F17" s="224" t="s">
         <v>200</v>
       </c>
-      <c r="G17" s="229"/>
+      <c r="G17" s="225"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5353,20 +5349,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="218" t="s">
         <v>203</v>
       </c>
-      <c r="C20" s="224"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="108" t="s">
         <v>201</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="237" t="s">
+      <c r="F20" s="233" t="s">
         <v>202</v>
       </c>
-      <c r="G20" s="238"/>
+      <c r="G20" s="234"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5408,14 +5404,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="242" t="s">
+      <c r="B22" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="243"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="215"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5440,17 +5436,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="232" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="224"/>
+      <c r="D23" s="219"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="237" t="s">
+      <c r="F23" s="233" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="238"/>
+      <c r="G23" s="234"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5594,10 +5590,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="210" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="211"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5624,8 +5620,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="239"/>
-      <c r="G29" s="240"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="211"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5964,7 +5960,7 @@
     </row>
     <row r="40" spans="2:26" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="216" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C40" s="217"/>
       <c r="D40" s="161">
@@ -5977,7 +5973,7 @@
         <v>205</v>
       </c>
       <c r="G40" s="160" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
@@ -6000,7 +5996,7 @@
     </row>
     <row r="41" spans="2:26" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="216" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C41" s="217"/>
       <c r="D41" s="161">
@@ -6013,7 +6009,7 @@
         <v>205</v>
       </c>
       <c r="G41" s="160" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
@@ -6036,7 +6032,7 @@
     </row>
     <row r="42" spans="2:26" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6049,7 +6045,7 @@
         <v>205</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6150,7 +6146,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6163,7 +6159,7 @@
         <v>205</v>
       </c>
       <c r="G46" s="160" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="18"/>
@@ -6186,7 +6182,7 @@
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
@@ -6199,7 +6195,7 @@
         <v>205</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6222,20 +6218,20 @@
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="216" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="C48" s="217"/>
       <c r="D48" s="161">
-        <v>45728</v>
+        <v>45743</v>
       </c>
       <c r="E48" s="161">
-        <v>45728</v>
+        <v>45743</v>
       </c>
       <c r="F48" s="160" t="s">
         <v>205</v>
       </c>
       <c r="G48" s="160" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
@@ -6294,7 +6290,7 @@
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="216" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C50" s="217"/>
       <c r="D50" s="161">
@@ -6307,7 +6303,7 @@
         <v>205</v>
       </c>
       <c r="G50" s="160" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
@@ -6382,7 +6378,7 @@
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="216" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C53" s="217"/>
       <c r="D53" s="161">
@@ -6395,7 +6391,7 @@
         <v>205</v>
       </c>
       <c r="G53" s="160" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H53" s="20"/>
       <c r="I53" s="18"/>
@@ -6418,7 +6414,7 @@
     </row>
     <row r="54" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="216" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C54" s="217"/>
       <c r="D54" s="161">
@@ -6503,14 +6499,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="219"/>
-      <c r="D57" s="219"/>
-      <c r="E57" s="219"/>
-      <c r="F57" s="219"/>
-      <c r="G57" s="220"/>
+      <c r="C57" s="242"/>
+      <c r="D57" s="242"/>
+      <c r="E57" s="242"/>
+      <c r="F57" s="242"/>
+      <c r="G57" s="243"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6769,9 +6765,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="232"/>
-      <c r="C66" s="232"/>
-      <c r="D66" s="232"/>
+      <c r="B66" s="228"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="228"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6796,11 +6792,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="232"/>
-      <c r="C67" s="232"/>
-      <c r="D67" s="232"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="234" t="s">
+      <c r="F67" s="230" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6825,10 +6821,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="233"/>
-      <c r="C68" s="233"/>
-      <c r="D68" s="233"/>
-      <c r="F68" s="235"/>
+      <c r="B68" s="229"/>
+      <c r="C68" s="229"/>
+      <c r="D68" s="229"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6851,11 +6847,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="241" t="s">
+      <c r="B69" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="241"/>
-      <c r="D69" s="241"/>
+      <c r="C69" s="212"/>
+      <c r="D69" s="212"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6907,11 +6903,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="230"/>
-      <c r="F71" s="221"/>
-      <c r="G71" s="221"/>
+      <c r="B71" s="226"/>
+      <c r="C71" s="226"/>
+      <c r="D71" s="226"/>
+      <c r="F71" s="244"/>
+      <c r="G71" s="244"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6933,11 +6929,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="231"/>
-      <c r="C72" s="231"/>
-      <c r="D72" s="231"/>
-      <c r="F72" s="222"/>
-      <c r="G72" s="222"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="F72" s="221"/>
+      <c r="G72" s="221"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6964,10 +6960,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="241" t="s">
+      <c r="F73" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="241"/>
+      <c r="G73" s="212"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7045,14 +7041,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="210" t="s">
+      <c r="B76" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="211"/>
-      <c r="D76" s="211"/>
-      <c r="E76" s="211"/>
-      <c r="F76" s="211"/>
-      <c r="G76" s="212"/>
+      <c r="C76" s="236"/>
+      <c r="D76" s="236"/>
+      <c r="E76" s="236"/>
+      <c r="F76" s="236"/>
+      <c r="G76" s="237"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7074,14 +7070,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="213" t="s">
+      <c r="B77" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="214"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="214"/>
-      <c r="F77" s="214"/>
-      <c r="G77" s="215"/>
+      <c r="C77" s="239"/>
+      <c r="D77" s="239"/>
+      <c r="E77" s="239"/>
+      <c r="F77" s="239"/>
+      <c r="G77" s="240"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7112,22 +7108,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7144,14 +7132,22 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7268,124 +7264,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="245"/>
+      <c r="P1" s="245"/>
+      <c r="Q1" s="245"/>
+      <c r="R1" s="245"/>
+      <c r="S1" s="245"/>
+      <c r="T1" s="245"/>
+      <c r="U1" s="245" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
+      <c r="V1" s="245"/>
+      <c r="W1" s="245"/>
+      <c r="X1" s="245"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="271"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="251" t="s">
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="245"/>
+      <c r="O2" s="245"/>
+      <c r="P2" s="245"/>
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="251"/>
-      <c r="W2" s="251"/>
-      <c r="X2" s="251"/>
+      <c r="V2" s="253"/>
+      <c r="W2" s="253"/>
+      <c r="X2" s="253"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="U3" s="254"/>
+      <c r="V3" s="254"/>
+      <c r="W3" s="254"/>
+      <c r="X3" s="254"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="250" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="276"/>
-      <c r="C4" s="276"/>
-      <c r="D4" s="276"/>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="276"/>
-      <c r="J4" s="276"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="275" t="s">
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="252"/>
+      <c r="N4" s="250" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="276"/>
-      <c r="T4" s="276"/>
-      <c r="U4" s="276"/>
-      <c r="V4" s="276"/>
-      <c r="W4" s="276"/>
-      <c r="X4" s="277"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="252"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="272"/>
-      <c r="B5" s="273"/>
-      <c r="C5" s="273"/>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="272"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="273"/>
-      <c r="X5" s="274"/>
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="247"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="248"/>
+      <c r="S5" s="248"/>
+      <c r="T5" s="248"/>
+      <c r="U5" s="248"/>
+      <c r="V5" s="248"/>
+      <c r="W5" s="248"/>
+      <c r="X5" s="249"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7414,66 +7410,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="249" t="s">
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="249"/>
-      <c r="L7" s="249"/>
-      <c r="M7" s="249"/>
-      <c r="N7" s="249"/>
-      <c r="O7" s="249"/>
-      <c r="P7" s="249" t="s">
+      <c r="K7" s="246"/>
+      <c r="L7" s="246"/>
+      <c r="M7" s="246"/>
+      <c r="N7" s="246"/>
+      <c r="O7" s="246"/>
+      <c r="P7" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="249"/>
-      <c r="R7" s="249"/>
-      <c r="S7" s="249"/>
-      <c r="T7" s="249"/>
-      <c r="U7" s="249"/>
-      <c r="V7" s="249"/>
-      <c r="W7" s="249"/>
-      <c r="X7" s="249"/>
+      <c r="Q7" s="246"/>
+      <c r="R7" s="246"/>
+      <c r="S7" s="246"/>
+      <c r="T7" s="246"/>
+      <c r="U7" s="246"/>
+      <c r="V7" s="246"/>
+      <c r="W7" s="246"/>
+      <c r="X7" s="246"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="256"/>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="257" t="s">
+      <c r="A8" s="255"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="255"/>
+      <c r="E8" s="255"/>
+      <c r="F8" s="255"/>
+      <c r="G8" s="255"/>
+      <c r="H8" s="255"/>
+      <c r="I8" s="255"/>
+      <c r="J8" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="258"/>
-      <c r="L8" s="258"/>
-      <c r="M8" s="258"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="259"/>
-      <c r="P8" s="257" t="s">
+      <c r="K8" s="257"/>
+      <c r="L8" s="257"/>
+      <c r="M8" s="257"/>
+      <c r="N8" s="257"/>
+      <c r="O8" s="258"/>
+      <c r="P8" s="256" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="258"/>
-      <c r="R8" s="258"/>
-      <c r="S8" s="258"/>
-      <c r="T8" s="258"/>
-      <c r="U8" s="258"/>
-      <c r="V8" s="258"/>
-      <c r="W8" s="258"/>
-      <c r="X8" s="259"/>
+      <c r="Q8" s="257"/>
+      <c r="R8" s="257"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
+      <c r="W8" s="257"/>
+      <c r="X8" s="258"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7502,66 +7498,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="269" t="s">
+      <c r="A10" s="259" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
-      <c r="M10" s="269"/>
-      <c r="N10" s="269"/>
-      <c r="O10" s="269"/>
-      <c r="P10" s="269"/>
-      <c r="Q10" s="269"/>
-      <c r="R10" s="269"/>
-      <c r="S10" s="269"/>
-      <c r="T10" s="269"/>
-      <c r="U10" s="269"/>
-      <c r="V10" s="269"/>
-      <c r="W10" s="269"/>
-      <c r="X10" s="269"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="259"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="259"/>
+      <c r="U10" s="259"/>
+      <c r="V10" s="259"/>
+      <c r="W10" s="259"/>
+      <c r="X10" s="259"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="260" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="270"/>
-      <c r="C11" s="270"/>
-      <c r="D11" s="270"/>
-      <c r="E11" s="270"/>
-      <c r="F11" s="270"/>
-      <c r="G11" s="270" t="s">
+      <c r="B11" s="260"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
+      <c r="E11" s="260"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="270"/>
-      <c r="I11" s="270"/>
-      <c r="J11" s="270"/>
-      <c r="K11" s="270"/>
-      <c r="L11" s="270"/>
-      <c r="M11" s="270" t="s">
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="270"/>
-      <c r="O11" s="270"/>
-      <c r="P11" s="270"/>
-      <c r="Q11" s="270"/>
-      <c r="R11" s="270"/>
-      <c r="S11" s="270" t="s">
+      <c r="N11" s="260"/>
+      <c r="O11" s="260"/>
+      <c r="P11" s="260"/>
+      <c r="Q11" s="260"/>
+      <c r="R11" s="260"/>
+      <c r="S11" s="260" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="270"/>
-      <c r="U11" s="270"/>
-      <c r="V11" s="270"/>
-      <c r="W11" s="270"/>
-      <c r="X11" s="270"/>
+      <c r="T11" s="260"/>
+      <c r="U11" s="260"/>
+      <c r="V11" s="260"/>
+      <c r="W11" s="260"/>
+      <c r="X11" s="260"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7590,66 +7586,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249" t="s">
+      <c r="A13" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249" t="s">
+      <c r="B13" s="246"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="249"/>
-      <c r="L13" s="249"/>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-      <c r="P13" s="249" t="s">
+      <c r="K13" s="246"/>
+      <c r="L13" s="246"/>
+      <c r="M13" s="246"/>
+      <c r="N13" s="246"/>
+      <c r="O13" s="246"/>
+      <c r="P13" s="246" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="249"/>
-      <c r="R13" s="249"/>
-      <c r="S13" s="249"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="249"/>
-      <c r="V13" s="249"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
+      <c r="Q13" s="246"/>
+      <c r="R13" s="246"/>
+      <c r="S13" s="246"/>
+      <c r="T13" s="246"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="246"/>
+      <c r="W13" s="246"/>
+      <c r="X13" s="246"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="256"/>
-      <c r="C14" s="256"/>
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
-      <c r="H14" s="256"/>
-      <c r="I14" s="256"/>
-      <c r="J14" s="257" t="s">
+      <c r="A14" s="255"/>
+      <c r="B14" s="255"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="255"/>
+      <c r="G14" s="255"/>
+      <c r="H14" s="255"/>
+      <c r="I14" s="255"/>
+      <c r="J14" s="256" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="258"/>
-      <c r="L14" s="258"/>
-      <c r="M14" s="258"/>
-      <c r="N14" s="258"/>
-      <c r="O14" s="259"/>
-      <c r="P14" s="257" t="s">
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
+      <c r="M14" s="257"/>
+      <c r="N14" s="257"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="256" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="258"/>
-      <c r="R14" s="258"/>
-      <c r="S14" s="258"/>
-      <c r="T14" s="258"/>
-      <c r="U14" s="258"/>
-      <c r="V14" s="258"/>
-      <c r="W14" s="258"/>
-      <c r="X14" s="259"/>
+      <c r="Q14" s="257"/>
+      <c r="R14" s="257"/>
+      <c r="S14" s="257"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
+      <c r="W14" s="257"/>
+      <c r="X14" s="258"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7678,184 +7674,172 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="266" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="260"/>
-      <c r="C16" s="260"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="260"/>
-      <c r="F16" s="260"/>
-      <c r="G16" s="260"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="260"/>
-      <c r="J16" s="261" t="s">
+      <c r="B16" s="266"/>
+      <c r="C16" s="266"/>
+      <c r="D16" s="266"/>
+      <c r="E16" s="266"/>
+      <c r="F16" s="266"/>
+      <c r="G16" s="266"/>
+      <c r="H16" s="266"/>
+      <c r="I16" s="266"/>
+      <c r="J16" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="261"/>
-      <c r="L16" s="261"/>
-      <c r="M16" s="261"/>
-      <c r="N16" s="260" t="s">
+      <c r="K16" s="267"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="267"/>
+      <c r="N16" s="266" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="260"/>
-      <c r="P16" s="260"/>
-      <c r="Q16" s="260"/>
-      <c r="R16" s="260"/>
-      <c r="S16" s="260"/>
-      <c r="T16" s="262" t="s">
+      <c r="O16" s="266"/>
+      <c r="P16" s="266"/>
+      <c r="Q16" s="266"/>
+      <c r="R16" s="266"/>
+      <c r="S16" s="266"/>
+      <c r="T16" s="268" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="262"/>
-      <c r="V16" s="262"/>
-      <c r="W16" s="262"/>
-      <c r="X16" s="262"/>
+      <c r="U16" s="268"/>
+      <c r="V16" s="268"/>
+      <c r="W16" s="268"/>
+      <c r="X16" s="268"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="261" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="C17" s="251"/>
-      <c r="D17" s="251"/>
-      <c r="E17" s="251"/>
-      <c r="F17" s="251"/>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="I17" s="252"/>
-      <c r="J17" s="263" t="s">
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="269" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="264"/>
-      <c r="L17" s="264"/>
-      <c r="M17" s="265"/>
-      <c r="N17" s="250" t="s">
+      <c r="K17" s="270"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="271"/>
+      <c r="N17" s="261" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="251"/>
-      <c r="P17" s="251"/>
-      <c r="Q17" s="251"/>
-      <c r="R17" s="251"/>
-      <c r="S17" s="252"/>
-      <c r="T17" s="250" t="s">
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="253"/>
+      <c r="S17" s="262"/>
+      <c r="T17" s="261" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="251"/>
-      <c r="V17" s="251"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
+      <c r="U17" s="253"/>
+      <c r="V17" s="253"/>
+      <c r="W17" s="253"/>
+      <c r="X17" s="262"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
-      <c r="B18" s="254"/>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="254"/>
-      <c r="G18" s="254"/>
-      <c r="H18" s="254"/>
-      <c r="I18" s="255"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="268"/>
-      <c r="N18" s="253"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
-      <c r="R18" s="254"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="253"/>
-      <c r="U18" s="254"/>
-      <c r="V18" s="254"/>
-      <c r="W18" s="254"/>
-      <c r="X18" s="255"/>
+      <c r="A18" s="263"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
+      <c r="J18" s="272"/>
+      <c r="K18" s="273"/>
+      <c r="L18" s="273"/>
+      <c r="M18" s="274"/>
+      <c r="N18" s="263"/>
+      <c r="O18" s="264"/>
+      <c r="P18" s="264"/>
+      <c r="Q18" s="264"/>
+      <c r="R18" s="264"/>
+      <c r="S18" s="265"/>
+      <c r="T18" s="263"/>
+      <c r="U18" s="264"/>
+      <c r="V18" s="264"/>
+      <c r="W18" s="264"/>
+      <c r="X18" s="265"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="248" t="s">
+      <c r="A21" s="278" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="248"/>
-      <c r="C21" s="248"/>
-      <c r="D21" s="248"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
-      <c r="G21" s="248"/>
-      <c r="H21" s="248"/>
+      <c r="B21" s="278"/>
+      <c r="C21" s="278"/>
+      <c r="D21" s="278"/>
+      <c r="E21" s="278"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="248" t="s">
+      <c r="J21" s="278" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
-      <c r="M21" s="248"/>
-      <c r="N21" s="248"/>
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
+      <c r="K21" s="278"/>
+      <c r="L21" s="278"/>
+      <c r="M21" s="278"/>
+      <c r="N21" s="278"/>
+      <c r="O21" s="278"/>
+      <c r="P21" s="278"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="248" t="s">
+      <c r="R21" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="248"/>
-      <c r="T21" s="248"/>
-      <c r="U21" s="248"/>
-      <c r="V21" s="248"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="248"/>
+      <c r="S21" s="278"/>
+      <c r="T21" s="278"/>
+      <c r="U21" s="278"/>
+      <c r="V21" s="278"/>
+      <c r="W21" s="278"/>
+      <c r="X21" s="278"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="245" t="s">
+      <c r="P23" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="245"/>
-      <c r="R23" s="245"/>
-      <c r="S23" s="245"/>
-      <c r="T23" s="245"/>
-      <c r="U23" s="246" t="s">
+      <c r="Q23" s="275"/>
+      <c r="R23" s="275"/>
+      <c r="S23" s="275"/>
+      <c r="T23" s="275"/>
+      <c r="U23" s="276" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="246"/>
-      <c r="W23" s="246"/>
-      <c r="X23" s="246"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="276"/>
+      <c r="X23" s="276"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="245" t="s">
+      <c r="P24" s="275" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="245"/>
-      <c r="U24" s="247" t="s">
+      <c r="Q24" s="275"/>
+      <c r="R24" s="275"/>
+      <c r="S24" s="275"/>
+      <c r="T24" s="275"/>
+      <c r="U24" s="277" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="247"/>
-      <c r="W24" s="247"/>
-      <c r="X24" s="247"/>
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7870,13 +7854,25 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
compatibilidad a post, barra de navegacion
</commit_message>
<xml_diff>
--- a/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva - copia.xlsx
+++ b/Bitacioras/GFPI-F-147V4FormatoBitacoraSeguimientoEtapaProductiva - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8E99E6-D186-42F7-9382-877E9580792E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D62FF9-95ED-4B0F-89F2-3435DDE1CCBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -874,19 +874,6 @@
     <t>SI</t>
   </si>
   <si>
-    <t>Comencé el día probando diferentes configuraciones y reorganizando el diseño. Comparé mi blog con otros, reubicando elementos a través de la interfaz de Blogger (que facilita este proceso), además de probar distintos colores y márgenes. Mejoré la disposición de las fechas y agregué un ícono para volver al menú principal. También eliminé temporalmente el carrusel de imágenes.
-Después de eso, mi tarea principal fue implementar una nueva forma de renderizar la página. Se trata de un sistema más avanzado que evita recargar toda la página al navegar entre pestañas, actualizando únicamente el contenido principal (main) mientras que el resto permanece estático.
-Cosas a destacar:
-No estoy completamente seguro de qué tan bien lo implementé.
-Es posible que cause inconvenientes en el futuro.
-Necesito hacer pruebas de rendimiento y compararlo con la versión anterior.
-Otra tarea en la que trabajé fue profundizar en la documentación y comprender mejor el código con las secciones incluidas. Finalmente, logré resolver el bug que hacía que el menú se abriera al cargar la página.</t>
-  </si>
-  <si>
-    <t>Para solucionar el problema del menú, tuve que encontrar la forma de agregar una clase a la etiqueta &lt;seccion-contents&gt;, la cual funciona como un incluible, es decir, se llama desde otra parte del código mediante &lt;macro:include&gt;.
-Y por fin comienzo a entender cómo se usa la etiqueta &lt;b:section-contents&gt;</t>
-  </si>
-  <si>
     <t>este dia no nos permitieron entrar a la oficina debido a una marcha que hubo a favor de los derecho laborales de los aprendices</t>
   </si>
   <si>
@@ -948,6 +935,13 @@
   <si>
     <t>Las secciones en Blogger funcionan de manera MUY extraña. Los widgets se guardan tanto en Blogger como en el código, por lo que para eliminarlos completamente, hay que hacerlo en ambos lugares.
 Encontrar un equilibrio entre llos estilos de las paginas indibiduales y los post, para que ambos se bean bien alavez que se dejen personalizar y no restrinjan tanto</t>
+  </si>
+  <si>
+    <t>actualize los post a los mas recientes, asi pude ver bug en el posicionamiento y maquilletodo un poco para que todo estuviera mas alineado, tambien cambie los tamaños un poco para que se vea mejor, cambie muchas cosas hacer cade su posiciona miento .
+agrege el menu de navegacion superior, y la pagina e practicas al blog todo responsivo para moviles, aun que cuando tenga mas pagina cambiare cosas de la visualizacion en movil</t>
+  </si>
+  <si>
+    <t>definitivamente el posiscionamieto de las imágenes, tuve que cambiar cosas con mucho cuidado para que no afectara a las paginas del blog, alfinal lo consegui pero definitivamente me costo mucho</t>
   </si>
 </sst>
 </file>
@@ -2803,6 +2797,39 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2815,6 +2842,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2866,77 +2932,92 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2956,99 +3037,87 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3067,83 +3136,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4130,56 +4124,56 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="175" t="s">
+      <c r="B5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4191,45 +4185,45 @@
       <c r="C8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="178" t="s">
+      <c r="D8" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="179"/>
+      <c r="E8" s="203"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="180" t="s">
+      <c r="B9" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="182"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="206"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="185"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="185" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="186"/>
+      <c r="E11" s="187"/>
     </row>
     <row r="12" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="166"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="179"/>
       <c r="F12" s="1"/>
       <c r="G12" s="35"/>
     </row>
@@ -4240,84 +4234,84 @@
       <c r="E13" s="76"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="198" t="s">
+      <c r="B14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="199"/>
-      <c r="D14" s="199"/>
-      <c r="E14" s="200"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="169"/>
     </row>
     <row r="15" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="201" t="s">
+      <c r="B15" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="203"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="172"/>
     </row>
     <row r="16" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="201" t="s">
+      <c r="B16" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="203"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="209"/>
+      <c r="C17" s="181"/>
+      <c r="D17" s="181"/>
+      <c r="E17" s="182"/>
     </row>
     <row r="18" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="203"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
     </row>
     <row r="19" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="201" t="s">
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
     </row>
     <row r="20" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="204" t="s">
+      <c r="B20" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="175"/>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="178"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187" t="s">
+      <c r="C22" s="186"/>
+      <c r="D22" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="188"/>
+      <c r="E22" s="187"/>
     </row>
     <row r="23" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="189"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="190"/>
-      <c r="E23" s="191"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190"/>
     </row>
     <row r="24" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
@@ -4326,10 +4320,10 @@
       <c r="C24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="192" t="s">
+      <c r="D24" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="192"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4339,8 +4333,8 @@
       <c r="C25" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
+      <c r="D25" s="183"/>
+      <c r="E25" s="184"/>
     </row>
     <row r="26" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="58" t="s">
@@ -4349,8 +4343,8 @@
       <c r="C26" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="194"/>
-      <c r="E26" s="195"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="60" t="s">
@@ -4359,8 +4353,8 @@
       <c r="C27" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="70" t="s">
@@ -4369,8 +4363,8 @@
       <c r="C28" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="195"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
     </row>
     <row r="29" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
@@ -4379,10 +4373,10 @@
       <c r="C29" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="194" t="s">
+      <c r="D29" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="195" t="s">
+      <c r="E29" s="184" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4393,10 +4387,10 @@
       <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="194" t="s">
+      <c r="D30" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="195" t="s">
+      <c r="E30" s="184" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4407,8 +4401,8 @@
       <c r="C31" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="194"/>
-      <c r="E31" s="195"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="184"/>
     </row>
     <row r="32" spans="2:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="70" t="s">
@@ -4417,10 +4411,10 @@
       <c r="C32" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="194" t="s">
+      <c r="D32" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="195" t="s">
+      <c r="E32" s="184" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4431,8 +4425,8 @@
       <c r="C33" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="184"/>
     </row>
     <row r="34" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="70" t="s">
@@ -4441,8 +4435,8 @@
       <c r="C34" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="194"/>
-      <c r="E34" s="195"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="184"/>
     </row>
     <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="70" t="s">
@@ -4451,8 +4445,8 @@
       <c r="C35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="194"/>
-      <c r="E35" s="195"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="184"/>
     </row>
     <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="70" t="s">
@@ -4461,8 +4455,8 @@
       <c r="C36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="194"/>
-      <c r="E36" s="195"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="184"/>
     </row>
     <row r="37" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="70" t="s">
@@ -4471,8 +4465,8 @@
       <c r="C37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="194"/>
-      <c r="E37" s="195"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="184"/>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="70" t="s">
@@ -4481,8 +4475,8 @@
       <c r="C38" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="194"/>
-      <c r="E38" s="195"/>
+      <c r="D38" s="183"/>
+      <c r="E38" s="184"/>
     </row>
     <row r="39" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="70" t="s">
@@ -4491,8 +4485,8 @@
       <c r="C39" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="184"/>
     </row>
     <row r="40" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="70" t="s">
@@ -4501,8 +4495,8 @@
       <c r="C40" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="194"/>
-      <c r="E40" s="195"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="184"/>
     </row>
     <row r="41" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="70" t="s">
@@ -4511,8 +4505,8 @@
       <c r="C41" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="194"/>
-      <c r="E41" s="195"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="184"/>
     </row>
     <row r="42" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" s="70" t="s">
@@ -4521,8 +4515,8 @@
       <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B43" s="70" t="s">
@@ -4531,10 +4525,10 @@
       <c r="C43" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="194" t="s">
+      <c r="D43" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="195" t="s">
+      <c r="E43" s="184" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4545,8 +4539,8 @@
       <c r="C44" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="194"/>
-      <c r="E44" s="195"/>
+      <c r="D44" s="183"/>
+      <c r="E44" s="184"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="70" t="s">
@@ -4555,8 +4549,8 @@
       <c r="C45" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="194"/>
-      <c r="E45" s="195"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="184"/>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="70" t="s">
@@ -4565,8 +4559,8 @@
       <c r="C46" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="194"/>
-      <c r="E46" s="195"/>
+      <c r="D46" s="183"/>
+      <c r="E46" s="184"/>
     </row>
     <row r="47" spans="2:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="70" t="s">
@@ -4575,10 +4569,10 @@
       <c r="C47" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="194" t="s">
+      <c r="D47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="195" t="s">
+      <c r="E47" s="184" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4589,8 +4583,8 @@
       <c r="C48" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="194"/>
-      <c r="E48" s="195"/>
+      <c r="D48" s="183"/>
+      <c r="E48" s="184"/>
     </row>
     <row r="49" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="70" t="s">
@@ -4599,10 +4593,10 @@
       <c r="C49" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="194" t="s">
+      <c r="D49" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="195" t="s">
+      <c r="E49" s="184" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4613,10 +4607,10 @@
       <c r="C50" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="194" t="s">
+      <c r="D50" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="195" t="s">
+      <c r="E50" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4627,10 +4621,10 @@
       <c r="C51" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="194" t="s">
+      <c r="D51" s="183" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="195" t="s">
+      <c r="E51" s="184" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4641,8 +4635,8 @@
       <c r="C52" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="194"/>
-      <c r="E52" s="195"/>
+      <c r="D52" s="183"/>
+      <c r="E52" s="184"/>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="70" t="s">
@@ -4651,8 +4645,8 @@
       <c r="C53" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="195"/>
+      <c r="D53" s="183"/>
+      <c r="E53" s="184"/>
     </row>
     <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
@@ -4661,8 +4655,8 @@
       <c r="C54" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="194"/>
-      <c r="E54" s="195"/>
+      <c r="D54" s="183"/>
+      <c r="E54" s="184"/>
     </row>
     <row r="55" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
@@ -4671,8 +4665,8 @@
       <c r="C55" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="195"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
     </row>
     <row r="56" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" s="71" t="s">
@@ -4681,8 +4675,8 @@
       <c r="C56" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="195"/>
+      <c r="D56" s="183"/>
+      <c r="E56" s="184"/>
     </row>
     <row r="57" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="72" t="s">
@@ -4691,10 +4685,10 @@
       <c r="C57" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="196" t="s">
+      <c r="D57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="197" t="s">
+      <c r="E57" s="166" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4712,6 +4706,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B19:E19"/>
@@ -4728,44 +4760,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4780,8 +4774,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4863,14 +4857,14 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
       <c r="H3" s="10"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4892,14 +4886,14 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="198"/>
       <c r="H4" s="10"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -4921,14 +4915,14 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="195"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
@@ -4950,14 +4944,14 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="198"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
@@ -4979,14 +4973,14 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="2:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="169" t="s">
+      <c r="B7" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="G7" s="195"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -5182,16 +5176,16 @@
       <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218">
+      <c r="B14" s="223">
         <v>2557356</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220" t="s">
+      <c r="C14" s="227"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="225" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="221"/>
-      <c r="G14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="226"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -5263,20 +5257,20 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="218" t="s">
+      <c r="B17" s="223" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="224"/>
       <c r="D17" s="120" t="s">
         <v>199</v>
       </c>
       <c r="E17" s="121">
         <v>7</v>
       </c>
-      <c r="F17" s="224" t="s">
+      <c r="F17" s="228" t="s">
         <v>200</v>
       </c>
-      <c r="G17" s="225"/>
+      <c r="G17" s="229"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="K17" s="20"/>
@@ -5344,20 +5338,20 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="218" t="s">
+      <c r="B20" s="223" t="s">
         <v>203</v>
       </c>
-      <c r="C20" s="219"/>
+      <c r="C20" s="224"/>
       <c r="D20" s="108" t="s">
         <v>201</v>
       </c>
       <c r="E20" s="116">
         <v>3177294629</v>
       </c>
-      <c r="F20" s="233" t="s">
+      <c r="F20" s="237" t="s">
         <v>202</v>
       </c>
-      <c r="G20" s="234"/>
+      <c r="G20" s="238"/>
       <c r="H20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -5399,14 +5393,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="242" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="214"/>
-      <c r="G22" s="215"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="243"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -5431,17 +5425,17 @@
       <c r="B23" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="236" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="219"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="233" t="s">
+      <c r="F23" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="234"/>
+      <c r="G23" s="238"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -5585,10 +5579,10 @@
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="211"/>
+      <c r="G28" s="240"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
@@ -5615,8 +5609,8 @@
       <c r="E29" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="210"/>
-      <c r="G29" s="211"/>
+      <c r="F29" s="239"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
@@ -5955,7 +5949,7 @@
     </row>
     <row r="40" spans="2:26" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="216" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C40" s="217"/>
       <c r="D40" s="161">
@@ -5968,7 +5962,7 @@
         <v>205</v>
       </c>
       <c r="G40" s="160" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
@@ -5991,7 +5985,7 @@
     </row>
     <row r="41" spans="2:26" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="216" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C41" s="217"/>
       <c r="D41" s="161">
@@ -6004,7 +5998,7 @@
         <v>205</v>
       </c>
       <c r="G41" s="160" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
@@ -6027,7 +6021,7 @@
     </row>
     <row r="42" spans="2:26" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="216" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C42" s="217"/>
       <c r="D42" s="161">
@@ -6040,7 +6034,7 @@
         <v>205</v>
       </c>
       <c r="G42" s="160" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -6141,7 +6135,7 @@
     </row>
     <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="216" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C46" s="217"/>
       <c r="D46" s="161">
@@ -6154,7 +6148,7 @@
         <v>205</v>
       </c>
       <c r="G46" s="160" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="18"/>
@@ -6177,7 +6171,7 @@
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
@@ -6190,7 +6184,7 @@
         <v>205</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6213,7 +6207,7 @@
     </row>
     <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="216" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C48" s="217"/>
       <c r="D48" s="161">
@@ -6226,7 +6220,7 @@
         <v>205</v>
       </c>
       <c r="G48" s="160" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
@@ -6249,7 +6243,7 @@
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="216" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C49" s="217"/>
       <c r="D49" s="161">
@@ -6262,7 +6256,7 @@
         <v>205</v>
       </c>
       <c r="G49" s="160" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
@@ -6337,7 +6331,7 @@
     </row>
     <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
@@ -6350,7 +6344,7 @@
         <v>205</v>
       </c>
       <c r="G52" s="160" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H52" s="20"/>
       <c r="I52" s="18"/>
@@ -6373,20 +6367,20 @@
     </row>
     <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="216" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="C53" s="217"/>
       <c r="D53" s="161">
-        <v>45733</v>
+        <v>45748</v>
       </c>
       <c r="E53" s="161">
-        <v>45733</v>
+        <v>45748</v>
       </c>
       <c r="F53" s="160" t="s">
         <v>205</v>
       </c>
       <c r="G53" s="160" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="H53" s="20"/>
       <c r="I53" s="18"/>
@@ -6409,7 +6403,7 @@
     </row>
     <row r="54" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="216" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C54" s="217"/>
       <c r="D54" s="161">
@@ -6494,14 +6488,14 @@
       <c r="Y56" s="22"/>
     </row>
     <row r="57" spans="2:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="241" t="s">
+      <c r="B57" s="218" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="243"/>
+      <c r="C57" s="219"/>
+      <c r="D57" s="219"/>
+      <c r="E57" s="219"/>
+      <c r="F57" s="219"/>
+      <c r="G57" s="220"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
       <c r="J57" s="29"/>
@@ -6760,9 +6754,9 @@
       <c r="Z65" s="18"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="228"/>
-      <c r="C66" s="228"/>
-      <c r="D66" s="228"/>
+      <c r="B66" s="232"/>
+      <c r="C66" s="232"/>
+      <c r="D66" s="232"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6787,11 +6781,11 @@
       <c r="Z66" s="18"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
+      <c r="B67" s="232"/>
+      <c r="C67" s="232"/>
+      <c r="D67" s="232"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="230" t="s">
+      <c r="F67" s="234" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="17"/>
@@ -6816,10 +6810,10 @@
       <c r="Z67" s="18"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="229"/>
-      <c r="C68" s="229"/>
-      <c r="D68" s="229"/>
-      <c r="F68" s="231"/>
+      <c r="B68" s="233"/>
+      <c r="C68" s="233"/>
+      <c r="D68" s="233"/>
+      <c r="F68" s="235"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
@@ -6842,11 +6836,11 @@
       <c r="Z68" s="18"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="212"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
       <c r="F69" s="19" t="s">
         <v>91</v>
       </c>
@@ -6898,11 +6892,11 @@
       <c r="Z70" s="18"/>
     </row>
     <row r="71" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="226"/>
-      <c r="C71" s="226"/>
-      <c r="D71" s="226"/>
-      <c r="F71" s="244"/>
-      <c r="G71" s="244"/>
+      <c r="B71" s="230"/>
+      <c r="C71" s="230"/>
+      <c r="D71" s="230"/>
+      <c r="F71" s="221"/>
+      <c r="G71" s="221"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
@@ -6924,11 +6918,11 @@
       <c r="Z71" s="18"/>
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="F72" s="221"/>
-      <c r="G72" s="221"/>
+      <c r="B72" s="231"/>
+      <c r="C72" s="231"/>
+      <c r="D72" s="231"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
       <c r="J72" s="18"/>
@@ -6955,10 +6949,10 @@
         <v>93</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="F73" s="212" t="s">
+      <c r="F73" s="241" t="s">
         <v>157</v>
       </c>
-      <c r="G73" s="212"/>
+      <c r="G73" s="241"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
@@ -7036,14 +7030,14 @@
       <c r="Z75" s="9"/>
     </row>
     <row r="76" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="235" t="s">
+      <c r="B76" s="210" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="236"/>
-      <c r="D76" s="236"/>
-      <c r="E76" s="236"/>
-      <c r="F76" s="236"/>
-      <c r="G76" s="237"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="211"/>
+      <c r="E76" s="211"/>
+      <c r="F76" s="211"/>
+      <c r="G76" s="212"/>
       <c r="H76" s="10"/>
       <c r="I76" s="36"/>
       <c r="J76" s="9"/>
@@ -7065,14 +7059,14 @@
       <c r="Z76" s="9"/>
     </row>
     <row r="77" spans="2:26" s="10" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="238" t="s">
+      <c r="B77" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="239"/>
-      <c r="D77" s="239"/>
-      <c r="E77" s="239"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="240"/>
+      <c r="C77" s="214"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="214"/>
+      <c r="F77" s="214"/>
+      <c r="G77" s="215"/>
     </row>
     <row r="78" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
@@ -7103,14 +7097,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B14:D14"/>
@@ -7127,22 +7129,14 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="F71:G72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{A401E140-5526-456E-AB09-9580EADBFEC9}"/>
@@ -7259,124 +7253,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="271" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="245"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="245"/>
-      <c r="S2" s="245"/>
-      <c r="T2" s="245"/>
-      <c r="U2" s="253" t="s">
+      <c r="A2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
+      <c r="K2" s="271"/>
+      <c r="L2" s="271"/>
+      <c r="M2" s="271"/>
+      <c r="N2" s="271"/>
+      <c r="O2" s="271"/>
+      <c r="P2" s="271"/>
+      <c r="Q2" s="271"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="251" t="s">
         <v>163</v>
       </c>
-      <c r="V2" s="253"/>
-      <c r="W2" s="253"/>
-      <c r="X2" s="253"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251"/>
+      <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
-      <c r="X3" s="254"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="250" t="s">
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="277"/>
+      <c r="N4" s="275" t="s">
         <v>165</v>
       </c>
-      <c r="O4" s="251"/>
-      <c r="P4" s="251"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="251"/>
-      <c r="S4" s="251"/>
-      <c r="T4" s="251"/>
-      <c r="U4" s="251"/>
-      <c r="V4" s="251"/>
-      <c r="W4" s="251"/>
-      <c r="X4" s="252"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="276"/>
+      <c r="Q4" s="276"/>
+      <c r="R4" s="276"/>
+      <c r="S4" s="276"/>
+      <c r="T4" s="276"/>
+      <c r="U4" s="276"/>
+      <c r="V4" s="276"/>
+      <c r="W4" s="276"/>
+      <c r="X4" s="277"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="247"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="248"/>
-      <c r="S5" s="248"/>
-      <c r="T5" s="248"/>
-      <c r="U5" s="248"/>
-      <c r="V5" s="248"/>
-      <c r="W5" s="248"/>
-      <c r="X5" s="249"/>
+      <c r="A5" s="272"/>
+      <c r="B5" s="273"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="273"/>
+      <c r="I5" s="273"/>
+      <c r="J5" s="273"/>
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="272"/>
+      <c r="O5" s="273"/>
+      <c r="P5" s="273"/>
+      <c r="Q5" s="273"/>
+      <c r="R5" s="273"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="273"/>
+      <c r="W5" s="273"/>
+      <c r="X5" s="274"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -7405,66 +7399,66 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
+      <c r="J7" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
-      <c r="M7" s="246"/>
-      <c r="N7" s="246"/>
-      <c r="O7" s="246"/>
-      <c r="P7" s="246" t="s">
+      <c r="K7" s="249"/>
+      <c r="L7" s="249"/>
+      <c r="M7" s="249"/>
+      <c r="N7" s="249"/>
+      <c r="O7" s="249"/>
+      <c r="P7" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="246"/>
-      <c r="R7" s="246"/>
-      <c r="S7" s="246"/>
-      <c r="T7" s="246"/>
-      <c r="U7" s="246"/>
-      <c r="V7" s="246"/>
-      <c r="W7" s="246"/>
-      <c r="X7" s="246"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="249"/>
+      <c r="U7" s="249"/>
+      <c r="V7" s="249"/>
+      <c r="W7" s="249"/>
+      <c r="X7" s="249"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="256" t="s">
+      <c r="A8" s="256"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="257" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="256" t="s">
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="259"/>
+      <c r="P8" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="257"/>
-      <c r="R8" s="257"/>
-      <c r="S8" s="257"/>
-      <c r="T8" s="257"/>
-      <c r="U8" s="257"/>
-      <c r="V8" s="257"/>
-      <c r="W8" s="257"/>
-      <c r="X8" s="258"/>
+      <c r="Q8" s="258"/>
+      <c r="R8" s="258"/>
+      <c r="S8" s="258"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="258"/>
+      <c r="V8" s="258"/>
+      <c r="W8" s="258"/>
+      <c r="X8" s="259"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -7493,66 +7487,66 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="269" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="259"/>
-      <c r="E10" s="259"/>
-      <c r="F10" s="259"/>
-      <c r="G10" s="259"/>
-      <c r="H10" s="259"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="259"/>
-      <c r="M10" s="259"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="259"/>
-      <c r="P10" s="259"/>
-      <c r="Q10" s="259"/>
-      <c r="R10" s="259"/>
-      <c r="S10" s="259"/>
-      <c r="T10" s="259"/>
-      <c r="U10" s="259"/>
-      <c r="V10" s="259"/>
-      <c r="W10" s="259"/>
-      <c r="X10" s="259"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
+      <c r="K10" s="269"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="269"/>
+      <c r="N10" s="269"/>
+      <c r="O10" s="269"/>
+      <c r="P10" s="269"/>
+      <c r="Q10" s="269"/>
+      <c r="R10" s="269"/>
+      <c r="S10" s="269"/>
+      <c r="T10" s="269"/>
+      <c r="U10" s="269"/>
+      <c r="V10" s="269"/>
+      <c r="W10" s="269"/>
+      <c r="X10" s="269"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="270" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="260"/>
-      <c r="C11" s="260"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="260"/>
-      <c r="G11" s="260" t="s">
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="270"/>
+      <c r="E11" s="270"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="260"/>
-      <c r="I11" s="260"/>
-      <c r="J11" s="260"/>
-      <c r="K11" s="260"/>
-      <c r="L11" s="260"/>
-      <c r="M11" s="260" t="s">
+      <c r="H11" s="270"/>
+      <c r="I11" s="270"/>
+      <c r="J11" s="270"/>
+      <c r="K11" s="270"/>
+      <c r="L11" s="270"/>
+      <c r="M11" s="270" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="260"/>
-      <c r="O11" s="260"/>
-      <c r="P11" s="260"/>
-      <c r="Q11" s="260"/>
-      <c r="R11" s="260"/>
-      <c r="S11" s="260" t="s">
+      <c r="N11" s="270"/>
+      <c r="O11" s="270"/>
+      <c r="P11" s="270"/>
+      <c r="Q11" s="270"/>
+      <c r="R11" s="270"/>
+      <c r="S11" s="270" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="260"/>
-      <c r="U11" s="260"/>
-      <c r="V11" s="260"/>
-      <c r="W11" s="260"/>
-      <c r="X11" s="260"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="270"/>
+      <c r="V11" s="270"/>
+      <c r="W11" s="270"/>
+      <c r="X11" s="270"/>
     </row>
     <row r="12" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -7581,66 +7575,66 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="246"/>
-      <c r="D13" s="246"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="246"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="246"/>
-      <c r="J13" s="246" t="s">
+      <c r="B13" s="249"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="246"/>
-      <c r="L13" s="246"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="246"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246" t="s">
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="249" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="246"/>
-      <c r="U13" s="246"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
+      <c r="Q13" s="249"/>
+      <c r="R13" s="249"/>
+      <c r="S13" s="249"/>
+      <c r="T13" s="249"/>
+      <c r="U13" s="249"/>
+      <c r="V13" s="249"/>
+      <c r="W13" s="249"/>
+      <c r="X13" s="249"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="255"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="255"/>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
-      <c r="F14" s="255"/>
-      <c r="G14" s="255"/>
-      <c r="H14" s="255"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="256" t="s">
+      <c r="A14" s="256"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="256"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="256"/>
+      <c r="F14" s="256"/>
+      <c r="G14" s="256"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="256"/>
+      <c r="J14" s="257" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="257"/>
-      <c r="L14" s="257"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="258"/>
-      <c r="P14" s="256" t="s">
+      <c r="K14" s="258"/>
+      <c r="L14" s="258"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="258"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="257" t="s">
         <v>175</v>
       </c>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="257"/>
-      <c r="U14" s="257"/>
-      <c r="V14" s="257"/>
-      <c r="W14" s="257"/>
-      <c r="X14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="258"/>
+      <c r="U14" s="258"/>
+      <c r="V14" s="258"/>
+      <c r="W14" s="258"/>
+      <c r="X14" s="259"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -7669,172 +7663,184 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:24" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="260" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="266"/>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="267" t="s">
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
+      <c r="G16" s="260"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="260"/>
+      <c r="J16" s="261" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="267"/>
-      <c r="L16" s="267"/>
-      <c r="M16" s="267"/>
-      <c r="N16" s="266" t="s">
+      <c r="K16" s="261"/>
+      <c r="L16" s="261"/>
+      <c r="M16" s="261"/>
+      <c r="N16" s="260" t="s">
         <v>178</v>
       </c>
-      <c r="O16" s="266"/>
-      <c r="P16" s="266"/>
-      <c r="Q16" s="266"/>
-      <c r="R16" s="266"/>
-      <c r="S16" s="266"/>
-      <c r="T16" s="268" t="s">
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="262" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="268"/>
-      <c r="V16" s="268"/>
-      <c r="W16" s="268"/>
-      <c r="X16" s="268"/>
+      <c r="U16" s="262"/>
+      <c r="V16" s="262"/>
+      <c r="W16" s="262"/>
+      <c r="X16" s="262"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="250" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="269" t="s">
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="263" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="270"/>
-      <c r="L17" s="270"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="261" t="s">
+      <c r="K17" s="264"/>
+      <c r="L17" s="264"/>
+      <c r="M17" s="265"/>
+      <c r="N17" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="Q17" s="253"/>
-      <c r="R17" s="253"/>
-      <c r="S17" s="262"/>
-      <c r="T17" s="261" t="s">
+      <c r="O17" s="251"/>
+      <c r="P17" s="251"/>
+      <c r="Q17" s="251"/>
+      <c r="R17" s="251"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="U17" s="253"/>
-      <c r="V17" s="253"/>
-      <c r="W17" s="253"/>
-      <c r="X17" s="262"/>
+      <c r="U17" s="251"/>
+      <c r="V17" s="251"/>
+      <c r="W17" s="251"/>
+      <c r="X17" s="252"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="265"/>
-      <c r="J18" s="272"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="274"/>
-      <c r="N18" s="263"/>
-      <c r="O18" s="264"/>
-      <c r="P18" s="264"/>
-      <c r="Q18" s="264"/>
-      <c r="R18" s="264"/>
-      <c r="S18" s="265"/>
-      <c r="T18" s="263"/>
-      <c r="U18" s="264"/>
-      <c r="V18" s="264"/>
-      <c r="W18" s="264"/>
-      <c r="X18" s="265"/>
+      <c r="A18" s="253"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="266"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="267"/>
+      <c r="M18" s="268"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="254"/>
+      <c r="P18" s="254"/>
+      <c r="Q18" s="254"/>
+      <c r="R18" s="254"/>
+      <c r="S18" s="255"/>
+      <c r="T18" s="253"/>
+      <c r="U18" s="254"/>
+      <c r="V18" s="254"/>
+      <c r="W18" s="254"/>
+      <c r="X18" s="255"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="248" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="278"/>
-      <c r="E21" s="278"/>
-      <c r="F21" s="278"/>
-      <c r="G21" s="278"/>
-      <c r="H21" s="278"/>
+      <c r="B21" s="248"/>
+      <c r="C21" s="248"/>
+      <c r="D21" s="248"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="278" t="s">
+      <c r="J21" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="278"/>
-      <c r="L21" s="278"/>
-      <c r="M21" s="278"/>
-      <c r="N21" s="278"/>
-      <c r="O21" s="278"/>
-      <c r="P21" s="278"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
+      <c r="M21" s="248"/>
+      <c r="N21" s="248"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="278" t="s">
+      <c r="R21" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="S21" s="278"/>
-      <c r="T21" s="278"/>
-      <c r="U21" s="278"/>
-      <c r="V21" s="278"/>
-      <c r="W21" s="278"/>
-      <c r="X21" s="278"/>
+      <c r="S21" s="248"/>
+      <c r="T21" s="248"/>
+      <c r="U21" s="248"/>
+      <c r="V21" s="248"/>
+      <c r="W21" s="248"/>
+      <c r="X21" s="248"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="275" t="s">
+      <c r="P23" s="245" t="s">
         <v>187</v>
       </c>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="276" t="s">
+      <c r="Q23" s="245"/>
+      <c r="R23" s="245"/>
+      <c r="S23" s="245"/>
+      <c r="T23" s="245"/>
+      <c r="U23" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="V23" s="276"/>
-      <c r="W23" s="276"/>
-      <c r="X23" s="276"/>
+      <c r="V23" s="246"/>
+      <c r="W23" s="246"/>
+      <c r="X23" s="246"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="275" t="s">
+      <c r="P24" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="277" t="s">
+      <c r="Q24" s="245"/>
+      <c r="R24" s="245"/>
+      <c r="S24" s="245"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="277"/>
-      <c r="W24" s="277"/>
-      <c r="X24" s="277"/>
+      <c r="V24" s="247"/>
+      <c r="W24" s="247"/>
+      <c r="X24" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:X23"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="R21:X21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="N4:X4"/>
+    <mergeCell ref="N5:X5"/>
+    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="P13:X13"/>
@@ -7849,25 +7855,13 @@
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="A17:I18"/>
     <mergeCell ref="J17:M18"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="N4:X4"/>
-    <mergeCell ref="N5:X5"/>
-    <mergeCell ref="U2:X3"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="P24:T24"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="R21:X21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="200" r:id="rId1"/>

</xml_diff>